<commit_message>
new hero and limiter
</commit_message>
<xml_diff>
--- a/opm_hero_property/heroes/13.xlsx
+++ b/opm_hero_property/heroes/13.xlsx
@@ -997,87 +997,87 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>21,1;31,1;41,1</t>
+          <t>21,56216;31,5728;41,2928</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>21,1;31,1;41,1</t>
+          <t>21,84262;31,0;41,4388</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>21,1;31,1;41,1</t>
+          <t>21,84262;31,0;41,0</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>21,1;31,1;41,1</t>
+          <t>21,6755;31,701;41,403</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>21,1;31,1;41,1</t>
+          <t>21,10125;31,0;41,603</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>21,1;31,1;41,1</t>
+          <t>21,10125;31,0;41,0</t>
         </is>
       </c>
       <c r="N2" t="n">
-        <v>1</v>
+        <v>56216.0235</v>
       </c>
       <c r="O2" t="n">
-        <v>1</v>
+        <v>5728.827200000001</v>
       </c>
       <c r="P2" t="n">
-        <v>1</v>
+        <v>2928.0873</v>
       </c>
       <c r="Q2" t="n">
-        <v>1</v>
+        <v>84262.2594</v>
       </c>
       <c r="R2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S2" t="n">
-        <v>1</v>
+        <v>4388.2059</v>
       </c>
       <c r="T2" t="n">
-        <v>1</v>
+        <v>84262.2594</v>
       </c>
       <c r="U2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W2" t="n">
-        <v>1</v>
+        <v>6755.112</v>
       </c>
       <c r="X2" t="n">
-        <v>1</v>
+        <v>701.1584</v>
       </c>
       <c r="Y2" t="n">
-        <v>1</v>
+        <v>403.0265</v>
       </c>
       <c r="Z2" t="n">
-        <v>1</v>
+        <v>10125.2448</v>
       </c>
       <c r="AA2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB2" t="n">
-        <v>1</v>
+        <v>603.9995</v>
       </c>
       <c r="AC2" t="n">
-        <v>1</v>
+        <v>10125.2448</v>
       </c>
       <c r="AD2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -1104,87 +1104,87 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>21,1;31,1;41,1</t>
+          <t>21,56221;31,5729;41,2928</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>21,1;31,1;41,1</t>
+          <t>21,84270;31,0;41,4388</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>21,1;31,1;41,1</t>
+          <t>21,84270;31,0;41,0</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>21,1;31,1;41,1</t>
+          <t>21,6760;31,702;41,403</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>21,1;31,1;41,1</t>
+          <t>21,10133;31,0;41,604</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>21,1;31,1;41,1</t>
+          <t>21,10133;31,0;41,0</t>
         </is>
       </c>
       <c r="N3" t="n">
-        <v>1</v>
+        <v>56221.256</v>
       </c>
       <c r="O3" t="n">
-        <v>1</v>
+        <v>5729.827600000001</v>
       </c>
       <c r="P3" t="n">
-        <v>1</v>
+        <v>2928.4976</v>
       </c>
       <c r="Q3" t="n">
-        <v>1</v>
+        <v>84270.10239999999</v>
       </c>
       <c r="R3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S3" t="n">
-        <v>1</v>
+        <v>4388.8208</v>
       </c>
       <c r="T3" t="n">
-        <v>1</v>
+        <v>84270.10239999999</v>
       </c>
       <c r="U3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W3" t="n">
-        <v>1</v>
+        <v>6760.3445</v>
       </c>
       <c r="X3" t="n">
-        <v>1</v>
+        <v>702.1588</v>
       </c>
       <c r="Y3" t="n">
-        <v>1</v>
+        <v>403.4368</v>
       </c>
       <c r="Z3" t="n">
-        <v>1</v>
+        <v>10133.0878</v>
       </c>
       <c r="AA3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB3" t="n">
-        <v>1</v>
+        <v>604.6143999999999</v>
       </c>
       <c r="AC3" t="n">
-        <v>1</v>
+        <v>10133.0878</v>
       </c>
       <c r="AD3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -1211,87 +1211,87 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>21,1;31,1;41,1</t>
+          <t>21,59697;31,6488;41,3331</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>21,1;31,1;41,1</t>
+          <t>21,89479;31,0;41,4992</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>21,1;31,1;41,1</t>
+          <t>21,89479;31,0;41,0</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>21,1;31,1;41,1</t>
+          <t>21,7134;31,783;41,448</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>21,1;31,1;41,1</t>
+          <t>21,10694;31,0;41,671</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>21,1;31,1;41,1</t>
+          <t>21,10694;31,0;41,0</t>
         </is>
       </c>
       <c r="N4" t="n">
-        <v>1</v>
+        <v>59697.0432877</v>
       </c>
       <c r="O4" t="n">
-        <v>1</v>
+        <v>6488.713401240001</v>
       </c>
       <c r="P4" t="n">
-        <v>1</v>
+        <v>3331.6298082</v>
       </c>
       <c r="Q4" t="n">
-        <v>1</v>
+        <v>89479.96378507999</v>
       </c>
       <c r="R4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S4" t="n">
-        <v>1</v>
+        <v>4992.9787206</v>
       </c>
       <c r="T4" t="n">
-        <v>1</v>
+        <v>89479.96378507999</v>
       </c>
       <c r="U4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W4" t="n">
-        <v>1</v>
+        <v>7134.932636649999</v>
       </c>
       <c r="X4" t="n">
-        <v>1</v>
+        <v>783.8176138800001</v>
       </c>
       <c r="Y4" t="n">
-        <v>1</v>
+        <v>448.0103746</v>
       </c>
       <c r="Z4" t="n">
-        <v>1</v>
+        <v>10694.55836966</v>
       </c>
       <c r="AA4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB4" t="n">
-        <v>1</v>
+        <v>671.4150118</v>
       </c>
       <c r="AC4" t="n">
-        <v>1</v>
+        <v>10694.55836966</v>
       </c>
       <c r="AD4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -1318,87 +1318,87 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>21,1;31,1;41,1</t>
+          <t>21,63637;31,7348;41,3788</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>21,1;31,1;41,1</t>
+          <t>21,95386;31,0;41,5677</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>21,1;31,1;41,1</t>
+          <t>21,95386;31,0;41,0</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>21,1;31,1;41,1</t>
+          <t>21,7559;31,876;41,498</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>21,1;31,1;41,1</t>
+          <t>21,11330;31,0;41,746</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>21,1;31,1;41,1</t>
+          <t>21,11330;31,0;41,0</t>
         </is>
       </c>
       <c r="N5" t="n">
-        <v>1</v>
+        <v>63637.7852838</v>
       </c>
       <c r="O5" t="n">
-        <v>1</v>
+        <v>7348.851248080001</v>
       </c>
       <c r="P5" t="n">
-        <v>1</v>
+        <v>3788.32147059</v>
       </c>
       <c r="Q5" t="n">
-        <v>1</v>
+        <v>95386.74629352</v>
       </c>
       <c r="R5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>1</v>
+        <v>5677.40402697</v>
       </c>
       <c r="T5" t="n">
-        <v>1</v>
+        <v>95386.74629352</v>
       </c>
       <c r="U5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W5" t="n">
-        <v>1</v>
+        <v>7559.0038251</v>
       </c>
       <c r="X5" t="n">
-        <v>1</v>
+        <v>876.2304349600001</v>
       </c>
       <c r="Y5" t="n">
-        <v>1</v>
+        <v>498.41975427</v>
       </c>
       <c r="Z5" t="n">
-        <v>1</v>
+        <v>11330.19914004</v>
       </c>
       <c r="AA5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB5" t="n">
-        <v>1</v>
+        <v>746.96150841</v>
       </c>
       <c r="AC5" t="n">
-        <v>1</v>
+        <v>11330.19914004</v>
       </c>
       <c r="AD5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -1425,87 +1425,87 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>21,52520;31,11992;41,4058</t>
+          <t>21,68276;31,8360;41,4325</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>21,52520;31,11992;41,4058</t>
+          <t>21,102339;31,0;41,6482</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>21,26260;31,5996;41,2029</t>
+          <t>21,102339;31,0;41,0</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>21,6198;31,1412;41,523</t>
+          <t>21,8057;31,984;41,557</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>21,6198;31,1412;41,523</t>
+          <t>21,12077;31,0;41,835</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>21,3099;31,706;41,261</t>
+          <t>21,12077;31,0;41,0</t>
         </is>
       </c>
       <c r="N6" t="n">
-        <v>52520</v>
+        <v>68276.50534249999</v>
       </c>
       <c r="O6" t="n">
-        <v>11992</v>
+        <v>8360.4875164</v>
       </c>
       <c r="P6" t="n">
-        <v>4058</v>
+        <v>4325.62465462</v>
       </c>
       <c r="Q6" t="n">
-        <v>52520</v>
+        <v>102339.728887</v>
       </c>
       <c r="R6" t="n">
-        <v>11992</v>
+        <v>0</v>
       </c>
       <c r="S6" t="n">
-        <v>4058</v>
+        <v>6482.63855746</v>
       </c>
       <c r="T6" t="n">
-        <v>26260</v>
+        <v>102339.728887</v>
       </c>
       <c r="U6" t="n">
-        <v>5996</v>
+        <v>0</v>
       </c>
       <c r="V6" t="n">
-        <v>2029</v>
+        <v>0</v>
       </c>
       <c r="W6" t="n">
-        <v>6198</v>
+        <v>8057.84559125</v>
       </c>
       <c r="X6" t="n">
-        <v>1412</v>
+        <v>984.8973868</v>
       </c>
       <c r="Y6" t="n">
-        <v>523</v>
+        <v>557.72892886</v>
       </c>
       <c r="Z6" t="n">
-        <v>6198</v>
+        <v>12077.9136115</v>
       </c>
       <c r="AA6" t="n">
-        <v>1412</v>
+        <v>0</v>
       </c>
       <c r="AB6" t="n">
-        <v>523</v>
+        <v>835.84576738</v>
       </c>
       <c r="AC6" t="n">
-        <v>3099</v>
+        <v>12077.9136115</v>
       </c>
       <c r="AD6" t="n">
-        <v>706</v>
+        <v>0</v>
       </c>
       <c r="AE6" t="n">
-        <v>261</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -1532,87 +1532,87 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>21,58299;31,13662;41,5112</t>
+          <t>21,75789;31,9525;41,5448</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>21,58299;31,13662;41,5112</t>
+          <t>21,113601;31,0;41,8165</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>21,29149;31,6831;41,2556</t>
+          <t>21,113601;31,0;41,0</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>21,6826;31,1594;41,640</t>
+          <t>21,8874;31,1111;41,682</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>21,6826;31,1594;41,640</t>
+          <t>21,13301;31,0;41,1022</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>21,3413;31,797;41,320</t>
+          <t>21,13301;31,0;41,0</t>
         </is>
       </c>
       <c r="N7" t="n">
-        <v>58299</v>
+        <v>75789.9694279</v>
       </c>
       <c r="O7" t="n">
-        <v>13662</v>
+        <v>9525.061806199999</v>
       </c>
       <c r="P7" t="n">
-        <v>5112</v>
+        <v>5448.23792054</v>
       </c>
       <c r="Q7" t="n">
-        <v>58299</v>
+        <v>113601.66846116</v>
       </c>
       <c r="R7" t="n">
-        <v>13662</v>
+        <v>0</v>
       </c>
       <c r="S7" t="n">
-        <v>5112</v>
+        <v>8165.05361282</v>
       </c>
       <c r="T7" t="n">
-        <v>29149</v>
+        <v>113601.66846116</v>
       </c>
       <c r="U7" t="n">
-        <v>6831</v>
+        <v>0</v>
       </c>
       <c r="V7" t="n">
-        <v>2556</v>
+        <v>0</v>
       </c>
       <c r="W7" t="n">
-        <v>6826</v>
+        <v>8874.302259549999</v>
       </c>
       <c r="X7" t="n">
-        <v>1594</v>
+        <v>1111.2580694</v>
       </c>
       <c r="Y7" t="n">
-        <v>640</v>
+        <v>682.4381666200001</v>
       </c>
       <c r="Z7" t="n">
-        <v>6826</v>
+        <v>13301.70140882</v>
       </c>
       <c r="AA7" t="n">
-        <v>1594</v>
+        <v>0</v>
       </c>
       <c r="AB7" t="n">
-        <v>640</v>
+        <v>1022.74245346</v>
       </c>
       <c r="AC7" t="n">
-        <v>3413</v>
+        <v>13301.70140882</v>
       </c>
       <c r="AD7" t="n">
-        <v>797</v>
+        <v>0</v>
       </c>
       <c r="AE7" t="n">
-        <v>320</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -1639,87 +1639,87 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>21,65774;31,15550;41,6569</t>
+          <t>21,85506;31,10841;41,7000</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>21,65774;31,15550;41,6569</t>
+          <t>21,128166;31,0;41,10491</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>21,32887;31,7775;41,3284</t>
+          <t>21,128166;31,0;41,0</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>21,7635;31,1797;41,801</t>
+          <t>21,9925;31,1253;41,854</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>21,7635;31,1797;41,801</t>
+          <t>21,14877;31,0;41,1280</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>21,3817;31,898;41,400</t>
+          <t>21,14877;31,0;41,0</t>
         </is>
       </c>
       <c r="N8" t="n">
-        <v>65774</v>
+        <v>85506.9792031</v>
       </c>
       <c r="O8" t="n">
-        <v>15550</v>
+        <v>10841.1115644</v>
       </c>
       <c r="P8" t="n">
-        <v>6569</v>
+        <v>7000.774362110001</v>
       </c>
       <c r="Q8" t="n">
-        <v>65774</v>
+        <v>128166.50509124</v>
       </c>
       <c r="R8" t="n">
-        <v>15550</v>
+        <v>0</v>
       </c>
       <c r="S8" t="n">
-        <v>6569</v>
+        <v>10491.77712713</v>
       </c>
       <c r="T8" t="n">
-        <v>32887</v>
+        <v>128166.50509124</v>
       </c>
       <c r="U8" t="n">
-        <v>7775</v>
+        <v>0</v>
       </c>
       <c r="V8" t="n">
-        <v>3284</v>
+        <v>0</v>
       </c>
       <c r="W8" t="n">
-        <v>7635</v>
+        <v>9925.760339949999</v>
       </c>
       <c r="X8" t="n">
-        <v>1797</v>
+        <v>1253.3471628</v>
       </c>
       <c r="Y8" t="n">
-        <v>801</v>
+        <v>854.52386883</v>
       </c>
       <c r="Z8" t="n">
-        <v>7635</v>
+        <v>14877.73308098</v>
       </c>
       <c r="AA8" t="n">
-        <v>1797</v>
+        <v>0</v>
       </c>
       <c r="AB8" t="n">
-        <v>801</v>
+        <v>1280.64032889</v>
       </c>
       <c r="AC8" t="n">
-        <v>3817</v>
+        <v>14877.73308098</v>
       </c>
       <c r="AD8" t="n">
-        <v>898</v>
+        <v>0</v>
       </c>
       <c r="AE8" t="n">
-        <v>400</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -1746,87 +1746,87 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>21,75382;31,17728;41,8529</t>
+          <t>21,97996;31,12359;41,9089</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>21,75382;31,17728;41,8529</t>
+          <t>21,146887;31,0;41,13622</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>21,37691;31,8864;41,4264</t>
+          <t>21,146887;31,0;41,0</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>21,8670;31,2031;41,1018</t>
+          <t>21,11272;31,1416;41,1085</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>21,8670;31,2031;41,1018</t>
+          <t>21,16895;31,0;41,1626</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>21,4335;31,1015;41,509</t>
+          <t>21,16895;31,0;41,0</t>
         </is>
       </c>
       <c r="N9" t="n">
-        <v>75382</v>
+        <v>97996.8387034</v>
       </c>
       <c r="O9" t="n">
-        <v>17728</v>
+        <v>12359.2750138</v>
       </c>
       <c r="P9" t="n">
-        <v>8529</v>
+        <v>9089.994707</v>
       </c>
       <c r="Q9" t="n">
-        <v>75382</v>
+        <v>146887.56922136</v>
       </c>
       <c r="R9" t="n">
-        <v>17728</v>
+        <v>0</v>
       </c>
       <c r="S9" t="n">
-        <v>8529</v>
+        <v>13622.807081</v>
       </c>
       <c r="T9" t="n">
-        <v>37691</v>
+        <v>146887.56922136</v>
       </c>
       <c r="U9" t="n">
-        <v>8864</v>
+        <v>0</v>
       </c>
       <c r="V9" t="n">
-        <v>4264</v>
+        <v>0</v>
       </c>
       <c r="W9" t="n">
-        <v>8670</v>
+        <v>11272.0764793</v>
       </c>
       <c r="X9" t="n">
-        <v>2031</v>
+        <v>1416.5538706</v>
       </c>
       <c r="Y9" t="n">
-        <v>1018</v>
+        <v>1085.551971</v>
       </c>
       <c r="Z9" t="n">
-        <v>8670</v>
+        <v>16895.72782172</v>
       </c>
       <c r="AA9" t="n">
-        <v>2031</v>
+        <v>0</v>
       </c>
       <c r="AB9" t="n">
-        <v>1018</v>
+        <v>1626.872793</v>
       </c>
       <c r="AC9" t="n">
-        <v>4335</v>
+        <v>16895.72782172</v>
       </c>
       <c r="AD9" t="n">
-        <v>1015</v>
+        <v>0</v>
       </c>
       <c r="AE9" t="n">
-        <v>509</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -1853,87 +1853,87 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>21,82584;31,18889;41,10162</t>
+          <t>21,107360;31,13168;41,10830</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>21,82584;31,18889;41,10162</t>
+          <t>21,160922;31,0;41,16230</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>21,41292;31,9444;41,5081</t>
+          <t>21,160922;31,0;41,0</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>21,9447;31,2156;41,1199</t>
+          <t>21,12281;31,1503;41,1278</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>21,9447;31,2156;41,1199</t>
+          <t>21,18408;31,0;41,1915</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>21,4723;31,1078;41,599</t>
+          <t>21,18408;31,0;41,0</t>
         </is>
       </c>
       <c r="N10" t="n">
-        <v>82584</v>
+        <v>107360.0819473</v>
       </c>
       <c r="O10" t="n">
-        <v>18889</v>
+        <v>13168.70143784</v>
       </c>
       <c r="P10" t="n">
-        <v>10162</v>
+        <v>10830.3213593</v>
       </c>
       <c r="Q10" t="n">
-        <v>82584</v>
+        <v>160922.14480892</v>
       </c>
       <c r="R10" t="n">
-        <v>18889</v>
+        <v>0</v>
       </c>
       <c r="S10" t="n">
-        <v>10162</v>
+        <v>16230.9641819</v>
       </c>
       <c r="T10" t="n">
-        <v>41292</v>
+        <v>160922.14480892</v>
       </c>
       <c r="U10" t="n">
-        <v>9444</v>
+        <v>0</v>
       </c>
       <c r="V10" t="n">
-        <v>5081</v>
+        <v>0</v>
       </c>
       <c r="W10" t="n">
-        <v>9447</v>
+        <v>12281.37177085</v>
       </c>
       <c r="X10" t="n">
-        <v>2156</v>
+        <v>1503.50428808</v>
       </c>
       <c r="Y10" t="n">
-        <v>1199</v>
+        <v>1278.0163529</v>
       </c>
       <c r="Z10" t="n">
-        <v>9447</v>
+        <v>18408.56164334</v>
       </c>
       <c r="AA10" t="n">
-        <v>2156</v>
+        <v>0</v>
       </c>
       <c r="AB10" t="n">
-        <v>1199</v>
+        <v>1915.3113707</v>
       </c>
       <c r="AC10" t="n">
-        <v>4723</v>
+        <v>18408.56164334</v>
       </c>
       <c r="AD10" t="n">
-        <v>1078</v>
+        <v>0</v>
       </c>
       <c r="AE10" t="n">
-        <v>599</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -1960,87 +1960,87 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>21,91367;31,20267;41,12166</t>
+          <t>21,118778;31,14129;41,12966</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>21,91367;31,20267;41,12166</t>
+          <t>21,178036;31,0;41,19432</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>21,45683;31,10133;41,6083</t>
+          <t>21,178036;31,0;41,0</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>21,10392;31,2304;41,1420</t>
+          <t>21,13510;31,1606;41,1513</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>21,10392;31,2304;41,1420</t>
+          <t>21,20250;31,0;41,2268</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>21,5196;31,1152;41,710</t>
+          <t>21,20250;31,0;41,0</t>
         </is>
       </c>
       <c r="N11" t="n">
-        <v>91367</v>
+        <v>118778.0581533</v>
       </c>
       <c r="O11" t="n">
-        <v>20267</v>
+        <v>14129.47988336</v>
       </c>
       <c r="P11" t="n">
-        <v>12166</v>
+        <v>12966.39230205</v>
       </c>
       <c r="Q11" t="n">
-        <v>91367</v>
+        <v>178036.56189132</v>
       </c>
       <c r="R11" t="n">
-        <v>20267</v>
+        <v>0</v>
       </c>
       <c r="S11" t="n">
-        <v>12166</v>
+        <v>19432.20723015</v>
       </c>
       <c r="T11" t="n">
-        <v>45683</v>
+        <v>178036.56189132</v>
       </c>
       <c r="U11" t="n">
-        <v>10133</v>
+        <v>0</v>
       </c>
       <c r="V11" t="n">
-        <v>6083</v>
+        <v>0</v>
       </c>
       <c r="W11" t="n">
-        <v>10392</v>
+        <v>13510.40020785</v>
       </c>
       <c r="X11" t="n">
-        <v>2304</v>
+        <v>1606.56243632</v>
       </c>
       <c r="Y11" t="n">
-        <v>1420</v>
+        <v>1513.97904365</v>
       </c>
       <c r="Z11" t="n">
-        <v>10392</v>
+        <v>20250.75371814</v>
       </c>
       <c r="AA11" t="n">
-        <v>2304</v>
+        <v>0</v>
       </c>
       <c r="AB11" t="n">
-        <v>1420</v>
+        <v>2268.93910295</v>
       </c>
       <c r="AC11" t="n">
-        <v>5196</v>
+        <v>20250.75371814</v>
       </c>
       <c r="AD11" t="n">
-        <v>1152</v>
+        <v>0</v>
       </c>
       <c r="AE11" t="n">
-        <v>710</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -2067,87 +2067,87 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>21,107549;31,23169;41,15734</t>
+          <t>21,139814;31,16152;41,16768</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>21,107549;31,23169;41,15734</t>
+          <t>21,209568;31,0;41,25129</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>21,53774;31,11584;41,7867</t>
+          <t>21,209568;31,0;41,0</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>21,12132;31,2615;41,1814</t>
+          <t>21,15771;31,1823;41,1933</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>21,12132;31,2615;41,1814</t>
+          <t>21,23640;31,0;41,2897</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>21,6066;31,1307;41,907</t>
+          <t>21,23640;31,0;41,0</t>
         </is>
       </c>
       <c r="N12" t="n">
-        <v>107549</v>
+        <v>139814.6533329</v>
       </c>
       <c r="O12" t="n">
-        <v>23169</v>
+        <v>16152.33762</v>
       </c>
       <c r="P12" t="n">
-        <v>15734</v>
+        <v>16768.02933179</v>
       </c>
       <c r="Q12" t="n">
-        <v>107549</v>
+        <v>209568.33752316</v>
       </c>
       <c r="R12" t="n">
-        <v>23169</v>
+        <v>0</v>
       </c>
       <c r="S12" t="n">
-        <v>15734</v>
+        <v>25129.56674657</v>
       </c>
       <c r="T12" t="n">
-        <v>53774</v>
+        <v>209568.33752316</v>
       </c>
       <c r="U12" t="n">
-        <v>11584</v>
+        <v>0</v>
       </c>
       <c r="V12" t="n">
-        <v>7867</v>
+        <v>0</v>
       </c>
       <c r="W12" t="n">
-        <v>12132</v>
+        <v>15771.63338205</v>
       </c>
       <c r="X12" t="n">
-        <v>2615</v>
+        <v>1823.48154</v>
       </c>
       <c r="Y12" t="n">
-        <v>1814</v>
+        <v>1933.54963787</v>
       </c>
       <c r="Z12" t="n">
-        <v>12132</v>
+        <v>23640.11860782</v>
       </c>
       <c r="AA12" t="n">
-        <v>2615</v>
+        <v>0</v>
       </c>
       <c r="AB12" t="n">
-        <v>1814</v>
+        <v>2897.73256721</v>
       </c>
       <c r="AC12" t="n">
-        <v>6066</v>
+        <v>23640.11860782</v>
       </c>
       <c r="AD12" t="n">
-        <v>1307</v>
+        <v>0</v>
       </c>
       <c r="AE12" t="n">
-        <v>907</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -2174,87 +2174,87 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>21,110053;31,23752;41,16239</t>
+          <t>21,143069;31,16558;41,17306</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>21,110053;31,23752;41,16239</t>
+          <t>21,214446;31,0;41,25936</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>21,55026;31,11876;41,8119</t>
+          <t>21,214446;31,0;41,0</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>21,12409;31,2679;41,1871</t>
+          <t>21,16132;31,1868;41,1994</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>21,12409;31,2679;41,1871</t>
+          <t>21,24181;31,0;41,2988</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>21,6204;31,1339;41,935</t>
+          <t>21,24181;31,0;41,0</t>
         </is>
       </c>
       <c r="N13" t="n">
-        <v>110053</v>
+        <v>143069.4292664</v>
       </c>
       <c r="O13" t="n">
-        <v>23752</v>
+        <v>16558.68635548</v>
       </c>
       <c r="P13" t="n">
-        <v>16239</v>
+        <v>17306.78721582</v>
       </c>
       <c r="Q13" t="n">
-        <v>110053</v>
+        <v>214446.92474656</v>
       </c>
       <c r="R13" t="n">
-        <v>23752</v>
+        <v>0</v>
       </c>
       <c r="S13" t="n">
-        <v>16239</v>
+        <v>25936.98137706</v>
       </c>
       <c r="T13" t="n">
-        <v>55026</v>
+        <v>214446.92474656</v>
       </c>
       <c r="U13" t="n">
-        <v>11876</v>
+        <v>0</v>
       </c>
       <c r="V13" t="n">
-        <v>8119</v>
+        <v>0</v>
       </c>
       <c r="W13" t="n">
-        <v>12409</v>
+        <v>16132.9459928</v>
       </c>
       <c r="X13" t="n">
-        <v>2679</v>
+        <v>1868.34088876</v>
       </c>
       <c r="Y13" t="n">
-        <v>1871</v>
+        <v>1994.31351246</v>
       </c>
       <c r="Z13" t="n">
-        <v>12409</v>
+        <v>24181.69047712</v>
       </c>
       <c r="AA13" t="n">
-        <v>2679</v>
+        <v>0</v>
       </c>
       <c r="AB13" t="n">
-        <v>1871</v>
+        <v>2988.79692618</v>
       </c>
       <c r="AC13" t="n">
-        <v>6204</v>
+        <v>24181.69047712</v>
       </c>
       <c r="AD13" t="n">
-        <v>1339</v>
+        <v>0</v>
       </c>
       <c r="AE13" t="n">
-        <v>935</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -2281,87 +2281,87 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>21,112561;31,24334;41,16745</t>
+          <t>21,146329;31,16964;41,17845</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>21,112561;31,24334;41,16745</t>
+          <t>21,219333;31,0;41,26744</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>21,56280;31,12167;41,8372</t>
+          <t>21,219333;31,0;41,0</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>21,12688;31,2744;41,1928</t>
+          <t>21,16494;31,1913;41,2055</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>21,12688;31,2744;41,1928</t>
+          <t>21,24724;31,0;41,3079</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>21,6344;31,1372;41,964</t>
+          <t>21,24724;31,0;41,0</t>
         </is>
       </c>
       <c r="N14" t="n">
-        <v>112561</v>
+        <v>146329.740375</v>
       </c>
       <c r="O14" t="n">
-        <v>24334</v>
+        <v>16964.49684404</v>
       </c>
       <c r="P14" t="n">
-        <v>16745</v>
+        <v>17845.82868056</v>
       </c>
       <c r="Q14" t="n">
-        <v>112561</v>
+        <v>219333.80865</v>
       </c>
       <c r="R14" t="n">
-        <v>24334</v>
+        <v>0</v>
       </c>
       <c r="S14" t="n">
-        <v>16745</v>
+        <v>26744.82099848</v>
       </c>
       <c r="T14" t="n">
-        <v>56280</v>
+        <v>219333.80865</v>
       </c>
       <c r="U14" t="n">
-        <v>12167</v>
+        <v>0</v>
       </c>
       <c r="V14" t="n">
-        <v>8372</v>
+        <v>0</v>
       </c>
       <c r="W14" t="n">
-        <v>12688</v>
+        <v>16494.8476875</v>
       </c>
       <c r="X14" t="n">
-        <v>2744</v>
+        <v>1913.16475748</v>
       </c>
       <c r="Y14" t="n">
-        <v>1928</v>
+        <v>2055.10846168</v>
       </c>
       <c r="Z14" t="n">
-        <v>12688</v>
+        <v>24724.145325</v>
       </c>
       <c r="AA14" t="n">
-        <v>2744</v>
+        <v>0</v>
       </c>
       <c r="AB14" t="n">
-        <v>1928</v>
+        <v>3079.90785544</v>
       </c>
       <c r="AC14" t="n">
-        <v>6344</v>
+        <v>24724.145325</v>
       </c>
       <c r="AD14" t="n">
-        <v>1372</v>
+        <v>0</v>
       </c>
       <c r="AE14" t="n">
-        <v>964</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -2388,87 +2388,87 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>21,115065;31,24917;41,17250</t>
+          <t>21,149584;31,17370;41,18384</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>21,115065;31,24917;41,17250</t>
+          <t>21,224212;31,0;41,27552</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>21,57532;31,12458;41,8625</t>
+          <t>21,224212;31,0;41,0</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>21,12966;31,2808;41,1985</t>
+          <t>21,16856;31,1958;41,2115</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>21,12966;31,2808;41,1985</t>
+          <t>21,25265;31,0;41,3171</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>21,6483;31,1404;41,992</t>
+          <t>21,25265;31,0;41,0</t>
         </is>
       </c>
       <c r="N15" t="n">
-        <v>115065</v>
+        <v>149584.5618085</v>
       </c>
       <c r="O15" t="n">
-        <v>24917</v>
+        <v>17370.84557952</v>
       </c>
       <c r="P15" t="n">
-        <v>17250</v>
+        <v>18384.62386459</v>
       </c>
       <c r="Q15" t="n">
-        <v>115065</v>
+        <v>224212.4640734</v>
       </c>
       <c r="R15" t="n">
-        <v>24917</v>
+        <v>0</v>
       </c>
       <c r="S15" t="n">
-        <v>17250</v>
+        <v>27552.29152897</v>
       </c>
       <c r="T15" t="n">
-        <v>57532</v>
+        <v>224212.4640734</v>
       </c>
       <c r="U15" t="n">
-        <v>12458</v>
+        <v>0</v>
       </c>
       <c r="V15" t="n">
-        <v>8625</v>
+        <v>0</v>
       </c>
       <c r="W15" t="n">
-        <v>12966</v>
+        <v>16856.20579825</v>
       </c>
       <c r="X15" t="n">
-        <v>2808</v>
+        <v>1958.02410624</v>
       </c>
       <c r="Y15" t="n">
-        <v>1985</v>
+        <v>2115.90963627</v>
       </c>
       <c r="Z15" t="n">
-        <v>12966</v>
+        <v>25265.7853943</v>
       </c>
       <c r="AA15" t="n">
-        <v>2808</v>
+        <v>0</v>
       </c>
       <c r="AB15" t="n">
-        <v>1985</v>
+        <v>3171.02811441</v>
       </c>
       <c r="AC15" t="n">
-        <v>6483</v>
+        <v>25265.7853943</v>
       </c>
       <c r="AD15" t="n">
-        <v>1404</v>
+        <v>0</v>
       </c>
       <c r="AE15" t="n">
-        <v>992</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -2495,87 +2495,87 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>21,117572;31,25499;41,17756</t>
+          <t>21,152844;31,17776;41,18923</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>21,117572;31,25499;41,17756</t>
+          <t>21,229099;31,0;41,28359</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>21,58786;31,12749;41,8878</t>
+          <t>21,229099;31,0;41,0</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>21,13244;31,2872;41,2042</t>
+          <t>21,17218;31,2002;41,2176</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>21,13244;31,2872;41,2042</t>
+          <t>21,25808;31,0;41,3262</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>21,6622;31,1436;41,1021</t>
+          <t>21,25808;31,0;41,0</t>
         </is>
       </c>
       <c r="N16" t="n">
-        <v>117572</v>
+        <v>152844.8729171</v>
       </c>
       <c r="O16" t="n">
-        <v>25499</v>
+        <v>17776.65606808</v>
       </c>
       <c r="P16" t="n">
-        <v>17756</v>
+        <v>18923.38174862</v>
       </c>
       <c r="Q16" t="n">
-        <v>117572</v>
+        <v>229099.34797684</v>
       </c>
       <c r="R16" t="n">
-        <v>25499</v>
+        <v>0</v>
       </c>
       <c r="S16" t="n">
-        <v>17756</v>
+        <v>28359.70615946</v>
       </c>
       <c r="T16" t="n">
-        <v>58786</v>
+        <v>229099.34797684</v>
       </c>
       <c r="U16" t="n">
-        <v>12749</v>
+        <v>0</v>
       </c>
       <c r="V16" t="n">
-        <v>8878</v>
+        <v>0</v>
       </c>
       <c r="W16" t="n">
-        <v>13244</v>
+        <v>17218.10749295</v>
       </c>
       <c r="X16" t="n">
-        <v>2872</v>
+        <v>2002.84797496</v>
       </c>
       <c r="Y16" t="n">
-        <v>2042</v>
+        <v>2176.67351086</v>
       </c>
       <c r="Z16" t="n">
-        <v>13244</v>
+        <v>25808.24024218</v>
       </c>
       <c r="AA16" t="n">
-        <v>2872</v>
+        <v>0</v>
       </c>
       <c r="AB16" t="n">
-        <v>2042</v>
+        <v>3262.09247338</v>
       </c>
       <c r="AC16" t="n">
-        <v>6622</v>
+        <v>25808.24024218</v>
       </c>
       <c r="AD16" t="n">
-        <v>1436</v>
+        <v>0</v>
       </c>
       <c r="AE16" t="n">
-        <v>1021</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -2602,87 +2602,87 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>21,120080;31,26081;41,18262</t>
+          <t>21,156105;31,18182;41,19462</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>21,120080;31,26081;41,18262</t>
+          <t>21,233986;31,0;41,29167</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>21,60040;31,13040;41,9131</t>
+          <t>21,233986;31,0;41,0</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>21,13523;31,2937;41,2099</t>
+          <t>21,17580;31,2047;41,2237</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>21,13523;31,2937;41,2099</t>
+          <t>21,26350;31,0;41,3353</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>21,6761;31,1468;41,1049</t>
+          <t>21,26350;31,0;41,0</t>
         </is>
       </c>
       <c r="N17" t="n">
-        <v>120080</v>
+        <v>156105.1840257</v>
       </c>
       <c r="O17" t="n">
-        <v>26081</v>
+        <v>18182.44215664</v>
       </c>
       <c r="P17" t="n">
-        <v>18262</v>
+        <v>19462.17693265</v>
       </c>
       <c r="Q17" t="n">
-        <v>120080</v>
+        <v>233986.23188028</v>
       </c>
       <c r="R17" t="n">
-        <v>26081</v>
+        <v>0</v>
       </c>
       <c r="S17" t="n">
-        <v>18262</v>
+        <v>29167.17668995</v>
       </c>
       <c r="T17" t="n">
-        <v>60040</v>
+        <v>233986.23188028</v>
       </c>
       <c r="U17" t="n">
-        <v>13040</v>
+        <v>0</v>
       </c>
       <c r="V17" t="n">
-        <v>9131</v>
+        <v>0</v>
       </c>
       <c r="W17" t="n">
-        <v>13523</v>
+        <v>17580.00918765</v>
       </c>
       <c r="X17" t="n">
-        <v>2937</v>
+        <v>2047.64744368</v>
       </c>
       <c r="Y17" t="n">
-        <v>2099</v>
+        <v>2237.47468545</v>
       </c>
       <c r="Z17" t="n">
-        <v>13523</v>
+        <v>26350.69509006</v>
       </c>
       <c r="AA17" t="n">
-        <v>2937</v>
+        <v>0</v>
       </c>
       <c r="AB17" t="n">
-        <v>2099</v>
+        <v>3353.21273235</v>
       </c>
       <c r="AC17" t="n">
-        <v>6761</v>
+        <v>26350.69509006</v>
       </c>
       <c r="AD17" t="n">
-        <v>1468</v>
+        <v>0</v>
       </c>
       <c r="AE17" t="n">
-        <v>1049</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -5107,141 +5107,141 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>7131</v>
+        <v>8741</v>
       </c>
       <c r="C2" t="n">
-        <v>1647</v>
+        <v>1022</v>
       </c>
       <c r="D2" t="n">
-        <v>768</v>
+        <v>1090</v>
       </c>
       <c r="E2" t="n">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="F2" t="n">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="G2" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H2" t="n">
-        <v>7131</v>
+        <v>11984</v>
       </c>
       <c r="I2" t="n">
-        <v>1647</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>768</v>
+        <v>1495</v>
       </c>
       <c r="K2" t="n">
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="L2" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="N2" t="n">
-        <v>3565</v>
+        <v>10445</v>
       </c>
       <c r="O2" t="n">
-        <v>823</v>
+        <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>384</v>
+        <v>0</v>
       </c>
       <c r="Q2" t="n">
-        <v>20</v>
+        <v>78</v>
       </c>
       <c r="R2" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="S2" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="T2" t="n">
-        <v>5003</v>
+        <v>4539</v>
       </c>
       <c r="U2" t="n">
-        <v>874</v>
+        <v>557</v>
       </c>
       <c r="V2" t="n">
-        <v>727</v>
+        <v>438</v>
       </c>
       <c r="W2" t="n">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="X2" t="n">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Y2" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="Z2" t="n">
-        <v>5003</v>
+        <v>6223</v>
       </c>
       <c r="AA2" t="n">
-        <v>874</v>
+        <v>0</v>
       </c>
       <c r="AB2" t="n">
-        <v>727</v>
+        <v>601</v>
       </c>
       <c r="AC2" t="n">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="AD2" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="AE2" t="n">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="AF2" t="n">
-        <v>2501</v>
+        <v>5424</v>
       </c>
       <c r="AG2" t="n">
-        <v>437</v>
+        <v>0</v>
       </c>
       <c r="AH2" t="n">
-        <v>363</v>
+        <v>0</v>
       </c>
       <c r="AI2" t="n">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="AJ2" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="AK2" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="AL2" t="inlineStr">
         <is>
-          <t>21,7131;31,1647;41,768;22,40;32,40;42,40</t>
+          <t>21,8741;31,1022;41,1090;22,52;32,28;42,42</t>
         </is>
       </c>
       <c r="AM2" t="inlineStr">
         <is>
-          <t>21,7131;31,1647;41,768;22,40;32,40;42,40</t>
+          <t>21,11984;31,0;41,1495;22,78;32,0;42,63</t>
         </is>
       </c>
       <c r="AN2" t="inlineStr">
         <is>
-          <t>21,3565;31,823;41,384;22,20;32,20;42,20</t>
+          <t>21,10445;31,0;41,0;22,78;32,0;42,0</t>
         </is>
       </c>
       <c r="AO2" t="inlineStr">
         <is>
-          <t>21,5003;31,874;41,727;22,35;32,35;42,35</t>
+          <t>21,4539;31,557;41,438;22,45;32,24;42,37</t>
         </is>
       </c>
       <c r="AP2" t="inlineStr">
         <is>
-          <t>21,5003;31,874;41,727;22,35;32,35;42,35</t>
+          <t>21,6223;31,0;41,601;22,68;32,0;42,55</t>
         </is>
       </c>
       <c r="AQ2" t="inlineStr">
         <is>
-          <t>21,2501;31,437;41,363;22,17;32,17;42,17</t>
+          <t>21,5424;31,0;41,0;22,66;32,0;42,0</t>
         </is>
       </c>
     </row>
@@ -5250,141 +5250,141 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>14299</v>
+        <v>17483</v>
       </c>
       <c r="C3" t="n">
-        <v>3179</v>
+        <v>2044</v>
       </c>
       <c r="D3" t="n">
-        <v>1645</v>
+        <v>2181</v>
       </c>
       <c r="E3" t="n">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="F3" t="n">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="G3" t="n">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="H3" t="n">
-        <v>14299</v>
+        <v>23969</v>
       </c>
       <c r="I3" t="n">
-        <v>3179</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>1645</v>
+        <v>2990</v>
       </c>
       <c r="K3" t="n">
-        <v>80</v>
+        <v>156</v>
       </c>
       <c r="L3" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>80</v>
+        <v>127</v>
       </c>
       <c r="N3" t="n">
-        <v>7149</v>
+        <v>20891</v>
       </c>
       <c r="O3" t="n">
-        <v>1589</v>
+        <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>822</v>
+        <v>0</v>
       </c>
       <c r="Q3" t="n">
-        <v>40</v>
+        <v>156</v>
       </c>
       <c r="R3" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="S3" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="T3" t="n">
-        <v>5241</v>
+        <v>5209</v>
       </c>
       <c r="U3" t="n">
-        <v>915</v>
+        <v>621</v>
       </c>
       <c r="V3" t="n">
-        <v>768</v>
+        <v>543</v>
       </c>
       <c r="W3" t="n">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="X3" t="n">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="Y3" t="n">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="Z3" t="n">
-        <v>5241</v>
+        <v>7142</v>
       </c>
       <c r="AA3" t="n">
-        <v>915</v>
+        <v>0</v>
       </c>
       <c r="AB3" t="n">
-        <v>768</v>
+        <v>745</v>
       </c>
       <c r="AC3" t="n">
-        <v>70</v>
+        <v>136</v>
       </c>
       <c r="AD3" t="n">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="AE3" t="n">
-        <v>70</v>
+        <v>111</v>
       </c>
       <c r="AF3" t="n">
-        <v>2620</v>
+        <v>6225</v>
       </c>
       <c r="AG3" t="n">
-        <v>457</v>
+        <v>0</v>
       </c>
       <c r="AH3" t="n">
-        <v>384</v>
+        <v>0</v>
       </c>
       <c r="AI3" t="n">
-        <v>35</v>
+        <v>136</v>
       </c>
       <c r="AJ3" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="AK3" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="AL3" t="inlineStr">
         <is>
-          <t>21,14299;31,3179;41,1645;22,80;32,80;42,80</t>
+          <t>21,17483;31,2044;41,2181;22,104;32,56;42,85</t>
         </is>
       </c>
       <c r="AM3" t="inlineStr">
         <is>
-          <t>21,14299;31,3179;41,1645;22,80;32,80;42,80</t>
+          <t>21,23969;31,0;41,2990;22,156;32,0;42,127</t>
         </is>
       </c>
       <c r="AN3" t="inlineStr">
         <is>
-          <t>21,7149;31,1589;41,822;22,40;32,40;42,40</t>
+          <t>21,20891;31,0;41,0;22,156;32,0;42,0</t>
         </is>
       </c>
       <c r="AO3" t="inlineStr">
         <is>
-          <t>21,5241;31,915;41,768;22,70;32,70;42,70</t>
+          <t>21,5209;31,621;41,543;22,91;32,49;42,74</t>
         </is>
       </c>
       <c r="AP3" t="inlineStr">
         <is>
-          <t>21,5241;31,915;41,768;22,70;32,70;42,70</t>
+          <t>21,7142;31,0;41,745;22,136;32,0;42,111</t>
         </is>
       </c>
       <c r="AQ3" t="inlineStr">
         <is>
-          <t>21,2620;31,457;41,384;22,35;32,35;42,35</t>
+          <t>21,6225;31,0;41,0;22,136;32,0;42,0</t>
         </is>
       </c>
     </row>
@@ -5393,141 +5393,141 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>21248</v>
+        <v>26225</v>
       </c>
       <c r="C4" t="n">
-        <v>4589</v>
+        <v>3066</v>
       </c>
       <c r="D4" t="n">
-        <v>2665</v>
+        <v>3272</v>
       </c>
       <c r="E4" t="n">
-        <v>120</v>
+        <v>156</v>
       </c>
       <c r="F4" t="n">
-        <v>120</v>
+        <v>84</v>
       </c>
       <c r="G4" t="n">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="H4" t="n">
-        <v>21248</v>
+        <v>35953</v>
       </c>
       <c r="I4" t="n">
-        <v>4589</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>2665</v>
+        <v>4485</v>
       </c>
       <c r="K4" t="n">
-        <v>120</v>
+        <v>234</v>
       </c>
       <c r="L4" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>120</v>
+        <v>191</v>
       </c>
       <c r="N4" t="n">
-        <v>10624</v>
+        <v>31337</v>
       </c>
       <c r="O4" t="n">
-        <v>2294</v>
+        <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>1332</v>
+        <v>0</v>
       </c>
       <c r="Q4" t="n">
-        <v>60</v>
+        <v>234</v>
       </c>
       <c r="R4" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="S4" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="T4" t="n">
-        <v>5490</v>
+        <v>6341</v>
       </c>
       <c r="U4" t="n">
-        <v>959</v>
+        <v>736</v>
       </c>
       <c r="V4" t="n">
-        <v>812</v>
+        <v>727</v>
       </c>
       <c r="W4" t="n">
-        <v>105</v>
+        <v>136</v>
       </c>
       <c r="X4" t="n">
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="Y4" t="n">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="Z4" t="n">
-        <v>5490</v>
+        <v>8693</v>
       </c>
       <c r="AA4" t="n">
-        <v>959</v>
+        <v>0</v>
       </c>
       <c r="AB4" t="n">
-        <v>812</v>
+        <v>997</v>
       </c>
       <c r="AC4" t="n">
-        <v>105</v>
+        <v>204</v>
       </c>
       <c r="AD4" t="n">
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="AE4" t="n">
-        <v>105</v>
+        <v>167</v>
       </c>
       <c r="AF4" t="n">
-        <v>2745</v>
+        <v>7577</v>
       </c>
       <c r="AG4" t="n">
-        <v>479</v>
+        <v>0</v>
       </c>
       <c r="AH4" t="n">
-        <v>406</v>
+        <v>0</v>
       </c>
       <c r="AI4" t="n">
-        <v>52</v>
+        <v>202</v>
       </c>
       <c r="AJ4" t="n">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="AK4" t="n">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="AL4" t="inlineStr">
         <is>
-          <t>21,21248;31,4589;41,2665;22,120;32,120;42,120</t>
+          <t>21,26225;31,3066;41,3272;22,156;32,84;42,127</t>
         </is>
       </c>
       <c r="AM4" t="inlineStr">
         <is>
-          <t>21,21248;31,4589;41,2665;22,120;32,120;42,120</t>
+          <t>21,35953;31,0;41,4485;22,234;32,0;42,191</t>
         </is>
       </c>
       <c r="AN4" t="inlineStr">
         <is>
-          <t>21,10624;31,2294;41,1332;22,60;32,60;42,60</t>
+          <t>21,31337;31,0;41,0;22,234;32,0;42,0</t>
         </is>
       </c>
       <c r="AO4" t="inlineStr">
         <is>
-          <t>21,5490;31,959;41,812;22,105;32,105;42,105</t>
+          <t>21,6341;31,736;41,727;22,136;32,73;42,111</t>
         </is>
       </c>
       <c r="AP4" t="inlineStr">
         <is>
-          <t>21,5490;31,959;41,812;22,105;32,105;42,105</t>
+          <t>21,8693;31,0;41,997;22,204;32,0;42,167</t>
         </is>
       </c>
       <c r="AQ4" t="inlineStr">
         <is>
-          <t>21,2745;31,479;41,406;22,52;32,52;42,52</t>
+          <t>21,7577;31,0;41,0;22,202;32,0;42,0</t>
         </is>
       </c>
     </row>
@@ -5536,141 +5536,141 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>28244</v>
+        <v>34967</v>
       </c>
       <c r="C5" t="n">
-        <v>6105</v>
+        <v>4089</v>
       </c>
       <c r="D5" t="n">
-        <v>3587</v>
+        <v>4362</v>
       </c>
       <c r="E5" t="n">
-        <v>160</v>
+        <v>208</v>
       </c>
       <c r="F5" t="n">
-        <v>160</v>
+        <v>112</v>
       </c>
       <c r="G5" t="n">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="H5" t="n">
-        <v>28244</v>
+        <v>47938</v>
       </c>
       <c r="I5" t="n">
-        <v>6105</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>3587</v>
+        <v>5981</v>
       </c>
       <c r="K5" t="n">
-        <v>160</v>
+        <v>312</v>
       </c>
       <c r="L5" t="n">
-        <v>160</v>
+        <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>160</v>
+        <v>255</v>
       </c>
       <c r="N5" t="n">
-        <v>14122</v>
+        <v>41783</v>
       </c>
       <c r="O5" t="n">
-        <v>3052</v>
+        <v>0</v>
       </c>
       <c r="P5" t="n">
-        <v>1793</v>
+        <v>0</v>
       </c>
       <c r="Q5" t="n">
-        <v>80</v>
+        <v>312</v>
       </c>
       <c r="R5" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="T5" t="n">
-        <v>5881</v>
+        <v>6793</v>
       </c>
       <c r="U5" t="n">
-        <v>1026</v>
+        <v>790</v>
       </c>
       <c r="V5" t="n">
-        <v>883</v>
+        <v>791</v>
       </c>
       <c r="W5" t="n">
-        <v>140</v>
+        <v>182</v>
       </c>
       <c r="X5" t="n">
-        <v>140</v>
+        <v>98</v>
       </c>
       <c r="Y5" t="n">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="Z5" t="n">
-        <v>5881</v>
+        <v>9313</v>
       </c>
       <c r="AA5" t="n">
-        <v>1026</v>
+        <v>0</v>
       </c>
       <c r="AB5" t="n">
-        <v>883</v>
+        <v>1085</v>
       </c>
       <c r="AC5" t="n">
-        <v>140</v>
+        <v>273</v>
       </c>
       <c r="AD5" t="n">
-        <v>140</v>
+        <v>0</v>
       </c>
       <c r="AE5" t="n">
-        <v>140</v>
+        <v>223</v>
       </c>
       <c r="AF5" t="n">
-        <v>2940</v>
+        <v>8117</v>
       </c>
       <c r="AG5" t="n">
-        <v>513</v>
+        <v>0</v>
       </c>
       <c r="AH5" t="n">
-        <v>441</v>
+        <v>0</v>
       </c>
       <c r="AI5" t="n">
-        <v>70</v>
+        <v>273</v>
       </c>
       <c r="AJ5" t="n">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="AK5" t="n">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="AL5" t="inlineStr">
         <is>
-          <t>21,28244;31,6105;41,3587;22,160;32,160;42,160</t>
+          <t>21,34967;31,4089;41,4362;22,208;32,112;42,170</t>
         </is>
       </c>
       <c r="AM5" t="inlineStr">
         <is>
-          <t>21,28244;31,6105;41,3587;22,160;32,160;42,160</t>
+          <t>21,47938;31,0;41,5981;22,312;32,0;42,255</t>
         </is>
       </c>
       <c r="AN5" t="inlineStr">
         <is>
-          <t>21,14122;31,3052;41,1793;22,80;32,80;42,80</t>
+          <t>21,41783;31,0;41,0;22,312;32,0;42,0</t>
         </is>
       </c>
       <c r="AO5" t="inlineStr">
         <is>
-          <t>21,5881;31,1026;41,883;22,140;32,140;42,140</t>
+          <t>21,6793;31,790;41,791;22,182;32,98;42,149</t>
         </is>
       </c>
       <c r="AP5" t="inlineStr">
         <is>
-          <t>21,5881;31,1026;41,883;22,140;32,140;42,140</t>
+          <t>21,9313;31,0;41,1085;22,273;32,0;42,223</t>
         </is>
       </c>
       <c r="AQ5" t="inlineStr">
         <is>
-          <t>21,2940;31,513;41,441;22,70;32,70;42,70</t>
+          <t>21,8117;31,0;41,0;22,273;32,0;42,0</t>
         </is>
       </c>
     </row>
@@ -5679,141 +5679,141 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>35204</v>
+        <v>43709</v>
       </c>
       <c r="C6" t="n">
-        <v>7618</v>
+        <v>5111</v>
       </c>
       <c r="D6" t="n">
-        <v>4525</v>
+        <v>5453</v>
       </c>
       <c r="E6" t="n">
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="F6" t="n">
-        <v>200</v>
+        <v>140</v>
       </c>
       <c r="G6" t="n">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="H6" t="n">
-        <v>35204</v>
+        <v>59923</v>
       </c>
       <c r="I6" t="n">
-        <v>7618</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>4525</v>
+        <v>7476</v>
       </c>
       <c r="K6" t="n">
-        <v>200</v>
+        <v>390</v>
       </c>
       <c r="L6" t="n">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>200</v>
+        <v>319</v>
       </c>
       <c r="N6" t="n">
-        <v>17602</v>
+        <v>52229</v>
       </c>
       <c r="O6" t="n">
-        <v>3809</v>
+        <v>0</v>
       </c>
       <c r="P6" t="n">
-        <v>2262</v>
+        <v>0</v>
       </c>
       <c r="Q6" t="n">
-        <v>100</v>
+        <v>390</v>
       </c>
       <c r="R6" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="S6" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="T6" t="n">
-        <v>6161</v>
+        <v>7274</v>
       </c>
       <c r="U6" t="n">
-        <v>1075</v>
+        <v>847</v>
       </c>
       <c r="V6" t="n">
-        <v>932</v>
+        <v>861</v>
       </c>
       <c r="W6" t="n">
-        <v>175</v>
+        <v>227</v>
       </c>
       <c r="X6" t="n">
-        <v>175</v>
+        <v>122</v>
       </c>
       <c r="Y6" t="n">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="Z6" t="n">
-        <v>6161</v>
+        <v>9973</v>
       </c>
       <c r="AA6" t="n">
-        <v>1075</v>
+        <v>0</v>
       </c>
       <c r="AB6" t="n">
-        <v>932</v>
+        <v>1180</v>
       </c>
       <c r="AC6" t="n">
-        <v>175</v>
+        <v>341</v>
       </c>
       <c r="AD6" t="n">
-        <v>175</v>
+        <v>0</v>
       </c>
       <c r="AE6" t="n">
-        <v>175</v>
+        <v>279</v>
       </c>
       <c r="AF6" t="n">
-        <v>3080</v>
+        <v>8693</v>
       </c>
       <c r="AG6" t="n">
-        <v>537</v>
+        <v>0</v>
       </c>
       <c r="AH6" t="n">
-        <v>466</v>
+        <v>0</v>
       </c>
       <c r="AI6" t="n">
-        <v>87</v>
+        <v>339</v>
       </c>
       <c r="AJ6" t="n">
-        <v>87</v>
+        <v>0</v>
       </c>
       <c r="AK6" t="n">
-        <v>87</v>
+        <v>0</v>
       </c>
       <c r="AL6" t="inlineStr">
         <is>
-          <t>21,35204;31,7618;41,4525;22,200;32,200;42,200</t>
+          <t>21,43709;31,5111;41,5453;22,260;32,140;42,213</t>
         </is>
       </c>
       <c r="AM6" t="inlineStr">
         <is>
-          <t>21,35204;31,7618;41,4525;22,200;32,200;42,200</t>
+          <t>21,59923;31,0;41,7476;22,390;32,0;42,319</t>
         </is>
       </c>
       <c r="AN6" t="inlineStr">
         <is>
-          <t>21,17602;31,3809;41,2262;22,100;32,100;42,100</t>
+          <t>21,52229;31,0;41,0;22,390;32,0;42,0</t>
         </is>
       </c>
       <c r="AO6" t="inlineStr">
         <is>
-          <t>21,6161;31,1075;41,932;22,175;32,175;42,175</t>
+          <t>21,7274;31,847;41,861;22,227;32,122;42,186</t>
         </is>
       </c>
       <c r="AP6" t="inlineStr">
         <is>
-          <t>21,6161;31,1075;41,932;22,175;32,175;42,175</t>
+          <t>21,9973;31,0;41,1180;22,341;32,0;42,279</t>
         </is>
       </c>
       <c r="AQ6" t="inlineStr">
         <is>
-          <t>21,3080;31,537;41,466;22,87;32,87;42,87</t>
+          <t>21,8693;31,0;41,0;22,339;32,0;42,0</t>
         </is>
       </c>
     </row>
@@ -5822,141 +5822,141 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>41019</v>
+        <v>52450</v>
       </c>
       <c r="C7" t="n">
-        <v>8886</v>
+        <v>6133</v>
       </c>
       <c r="D7" t="n">
-        <v>5868</v>
+        <v>6544</v>
       </c>
       <c r="E7" t="n">
-        <v>240</v>
+        <v>312</v>
       </c>
       <c r="F7" t="n">
-        <v>240</v>
+        <v>168</v>
       </c>
       <c r="G7" t="n">
-        <v>240</v>
+        <v>255</v>
       </c>
       <c r="H7" t="n">
-        <v>41019</v>
+        <v>71907</v>
       </c>
       <c r="I7" t="n">
-        <v>8886</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
-        <v>5868</v>
+        <v>8971</v>
       </c>
       <c r="K7" t="n">
-        <v>240</v>
+        <v>468</v>
       </c>
       <c r="L7" t="n">
-        <v>240</v>
+        <v>0</v>
       </c>
       <c r="M7" t="n">
-        <v>240</v>
+        <v>383</v>
       </c>
       <c r="N7" t="n">
-        <v>20509</v>
+        <v>62675</v>
       </c>
       <c r="O7" t="n">
-        <v>4443</v>
+        <v>0</v>
       </c>
       <c r="P7" t="n">
-        <v>2934</v>
+        <v>0</v>
       </c>
       <c r="Q7" t="n">
-        <v>120</v>
+        <v>468</v>
       </c>
       <c r="R7" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="S7" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="T7" t="n">
-        <v>6454</v>
+        <v>7787</v>
       </c>
       <c r="U7" t="n">
-        <v>1126</v>
+        <v>908</v>
       </c>
       <c r="V7" t="n">
-        <v>984</v>
+        <v>935</v>
       </c>
       <c r="W7" t="n">
-        <v>210</v>
+        <v>273</v>
       </c>
       <c r="X7" t="n">
-        <v>210</v>
+        <v>147</v>
       </c>
       <c r="Y7" t="n">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="Z7" t="n">
-        <v>6454</v>
+        <v>10675</v>
       </c>
       <c r="AA7" t="n">
-        <v>1126</v>
+        <v>0</v>
       </c>
       <c r="AB7" t="n">
-        <v>984</v>
+        <v>1282</v>
       </c>
       <c r="AC7" t="n">
-        <v>210</v>
+        <v>409</v>
       </c>
       <c r="AD7" t="n">
-        <v>210</v>
+        <v>0</v>
       </c>
       <c r="AE7" t="n">
-        <v>210</v>
+        <v>335</v>
       </c>
       <c r="AF7" t="n">
-        <v>3227</v>
+        <v>9305</v>
       </c>
       <c r="AG7" t="n">
-        <v>563</v>
+        <v>0</v>
       </c>
       <c r="AH7" t="n">
-        <v>492</v>
+        <v>0</v>
       </c>
       <c r="AI7" t="n">
-        <v>105</v>
+        <v>409</v>
       </c>
       <c r="AJ7" t="n">
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="AK7" t="n">
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="AL7" t="inlineStr">
         <is>
-          <t>21,41019;31,8886;41,5868;22,240;32,240;42,240</t>
+          <t>21,52450;31,6133;41,6544;22,312;32,168;42,255</t>
         </is>
       </c>
       <c r="AM7" t="inlineStr">
         <is>
-          <t>21,41019;31,8886;41,5868;22,240;32,240;42,240</t>
+          <t>21,71907;31,0;41,8971;22,468;32,0;42,383</t>
         </is>
       </c>
       <c r="AN7" t="inlineStr">
         <is>
-          <t>21,20509;31,4443;41,2934;22,120;32,120;42,120</t>
+          <t>21,62675;31,0;41,0;22,468;32,0;42,0</t>
         </is>
       </c>
       <c r="AO7" t="inlineStr">
         <is>
-          <t>21,6454;31,1126;41,984;22,210;32,210;42,210</t>
+          <t>21,7787;31,908;41,935;22,273;32,147;42,223</t>
         </is>
       </c>
       <c r="AP7" t="inlineStr">
         <is>
-          <t>21,6454;31,1126;41,984;22,210;32,210;42,210</t>
+          <t>21,10675;31,0;41,1282;22,409;32,0;42,335</t>
         </is>
       </c>
       <c r="AQ7" t="inlineStr">
         <is>
-          <t>21,3227;31,563;41,492;22,105;32,105;42,105</t>
+          <t>21,9305;31,0;41,0;22,409;32,0;42,0</t>
         </is>
       </c>
     </row>
@@ -5965,141 +5965,141 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>46810</v>
+        <v>61192</v>
       </c>
       <c r="C8" t="n">
-        <v>10153</v>
+        <v>7156</v>
       </c>
       <c r="D8" t="n">
-        <v>7218</v>
+        <v>7634</v>
       </c>
       <c r="E8" t="n">
-        <v>280</v>
+        <v>364</v>
       </c>
       <c r="F8" t="n">
-        <v>280</v>
+        <v>196</v>
       </c>
       <c r="G8" t="n">
-        <v>280</v>
+        <v>298</v>
       </c>
       <c r="H8" t="n">
-        <v>46810</v>
+        <v>83892</v>
       </c>
       <c r="I8" t="n">
-        <v>10153</v>
+        <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>7218</v>
+        <v>10467</v>
       </c>
       <c r="K8" t="n">
-        <v>280</v>
+        <v>546</v>
       </c>
       <c r="L8" t="n">
-        <v>280</v>
+        <v>0</v>
       </c>
       <c r="M8" t="n">
-        <v>280</v>
+        <v>447</v>
       </c>
       <c r="N8" t="n">
-        <v>23405</v>
+        <v>73121</v>
       </c>
       <c r="O8" t="n">
-        <v>5076</v>
+        <v>0</v>
       </c>
       <c r="P8" t="n">
-        <v>3609</v>
+        <v>0</v>
       </c>
       <c r="Q8" t="n">
-        <v>140</v>
+        <v>546</v>
       </c>
       <c r="R8" t="n">
-        <v>140</v>
+        <v>0</v>
       </c>
       <c r="S8" t="n">
-        <v>140</v>
+        <v>0</v>
       </c>
       <c r="T8" t="n">
-        <v>6762</v>
+        <v>8332</v>
       </c>
       <c r="U8" t="n">
-        <v>1179</v>
+        <v>973</v>
       </c>
       <c r="V8" t="n">
-        <v>1038</v>
+        <v>1015</v>
       </c>
       <c r="W8" t="n">
-        <v>245</v>
+        <v>318</v>
       </c>
       <c r="X8" t="n">
-        <v>245</v>
+        <v>171</v>
       </c>
       <c r="Y8" t="n">
-        <v>245</v>
+        <v>261</v>
       </c>
       <c r="Z8" t="n">
-        <v>6762</v>
+        <v>11423</v>
       </c>
       <c r="AA8" t="n">
-        <v>1179</v>
+        <v>0</v>
       </c>
       <c r="AB8" t="n">
-        <v>1038</v>
+        <v>1392</v>
       </c>
       <c r="AC8" t="n">
-        <v>245</v>
+        <v>477</v>
       </c>
       <c r="AD8" t="n">
-        <v>245</v>
+        <v>0</v>
       </c>
       <c r="AE8" t="n">
-        <v>245</v>
+        <v>391</v>
       </c>
       <c r="AF8" t="n">
-        <v>3381</v>
+        <v>9956</v>
       </c>
       <c r="AG8" t="n">
-        <v>589</v>
+        <v>0</v>
       </c>
       <c r="AH8" t="n">
-        <v>519</v>
+        <v>0</v>
       </c>
       <c r="AI8" t="n">
-        <v>122</v>
+        <v>475</v>
       </c>
       <c r="AJ8" t="n">
-        <v>122</v>
+        <v>0</v>
       </c>
       <c r="AK8" t="n">
-        <v>122</v>
+        <v>0</v>
       </c>
       <c r="AL8" t="inlineStr">
         <is>
-          <t>21,46810;31,10153;41,7218;22,280;32,280;42,280</t>
+          <t>21,61192;31,7156;41,7634;22,364;32,196;42,298</t>
         </is>
       </c>
       <c r="AM8" t="inlineStr">
         <is>
-          <t>21,46810;31,10153;41,7218;22,280;32,280;42,280</t>
+          <t>21,83892;31,0;41,10467;22,546;32,0;42,447</t>
         </is>
       </c>
       <c r="AN8" t="inlineStr">
         <is>
-          <t>21,23405;31,5076;41,3609;22,140;32,140;42,140</t>
+          <t>21,73121;31,0;41,0;22,546;32,0;42,0</t>
         </is>
       </c>
       <c r="AO8" t="inlineStr">
         <is>
-          <t>21,6762;31,1179;41,1038;22,245;32,245;42,245</t>
+          <t>21,8332;31,973;41,1015;22,318;32,171;42,261</t>
         </is>
       </c>
       <c r="AP8" t="inlineStr">
         <is>
-          <t>21,6762;31,1179;41,1038;22,245;32,245;42,245</t>
+          <t>21,11423;31,0;41,1392;22,477;32,0;42,391</t>
         </is>
       </c>
       <c r="AQ8" t="inlineStr">
         <is>
-          <t>21,3381;31,589;41,519;22,122;32,122;42,122</t>
+          <t>21,9956;31,0;41,0;22,475;32,0;42,0</t>
         </is>
       </c>
     </row>
@@ -6108,141 +6108,141 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>53038</v>
+        <v>69934</v>
       </c>
       <c r="C9" t="n">
-        <v>11519</v>
+        <v>8178</v>
       </c>
       <c r="D9" t="n">
-        <v>8413</v>
+        <v>8725</v>
       </c>
       <c r="E9" t="n">
-        <v>315</v>
+        <v>409</v>
       </c>
       <c r="F9" t="n">
-        <v>315</v>
+        <v>220</v>
       </c>
       <c r="G9" t="n">
-        <v>315</v>
+        <v>335</v>
       </c>
       <c r="H9" t="n">
-        <v>53038</v>
+        <v>95876</v>
       </c>
       <c r="I9" t="n">
-        <v>11519</v>
+        <v>0</v>
       </c>
       <c r="J9" t="n">
-        <v>8413</v>
+        <v>11962</v>
       </c>
       <c r="K9" t="n">
-        <v>315</v>
+        <v>614</v>
       </c>
       <c r="L9" t="n">
-        <v>315</v>
+        <v>0</v>
       </c>
       <c r="M9" t="n">
-        <v>315</v>
+        <v>503</v>
       </c>
       <c r="N9" t="n">
-        <v>26519</v>
+        <v>83567</v>
       </c>
       <c r="O9" t="n">
-        <v>5759</v>
+        <v>0</v>
       </c>
       <c r="P9" t="n">
-        <v>4206</v>
+        <v>0</v>
       </c>
       <c r="Q9" t="n">
-        <v>157</v>
+        <v>612</v>
       </c>
       <c r="R9" t="n">
-        <v>157</v>
+        <v>0</v>
       </c>
       <c r="S9" t="n">
-        <v>157</v>
+        <v>0</v>
       </c>
       <c r="T9" t="n">
-        <v>7353</v>
+        <v>9251</v>
       </c>
       <c r="U9" t="n">
-        <v>1283</v>
+        <v>1081</v>
       </c>
       <c r="V9" t="n">
-        <v>1144</v>
+        <v>1150</v>
       </c>
       <c r="W9" t="n">
-        <v>280</v>
+        <v>364</v>
       </c>
       <c r="X9" t="n">
-        <v>280</v>
+        <v>196</v>
       </c>
       <c r="Y9" t="n">
-        <v>280</v>
+        <v>298</v>
       </c>
       <c r="Z9" t="n">
-        <v>7353</v>
+        <v>12682</v>
       </c>
       <c r="AA9" t="n">
-        <v>1283</v>
+        <v>0</v>
       </c>
       <c r="AB9" t="n">
-        <v>1144</v>
+        <v>1577</v>
       </c>
       <c r="AC9" t="n">
-        <v>280</v>
+        <v>546</v>
       </c>
       <c r="AD9" t="n">
-        <v>280</v>
+        <v>0</v>
       </c>
       <c r="AE9" t="n">
-        <v>280</v>
+        <v>447</v>
       </c>
       <c r="AF9" t="n">
-        <v>3676</v>
+        <v>11054</v>
       </c>
       <c r="AG9" t="n">
-        <v>641</v>
+        <v>0</v>
       </c>
       <c r="AH9" t="n">
-        <v>572</v>
+        <v>0</v>
       </c>
       <c r="AI9" t="n">
-        <v>140</v>
+        <v>546</v>
       </c>
       <c r="AJ9" t="n">
-        <v>140</v>
+        <v>0</v>
       </c>
       <c r="AK9" t="n">
-        <v>140</v>
+        <v>0</v>
       </c>
       <c r="AL9" t="inlineStr">
         <is>
-          <t>21,53038;31,11519;41,8413;22,315;32,315;42,315</t>
+          <t>21,69934;31,8178;41,8725;22,409;32,220;42,335</t>
         </is>
       </c>
       <c r="AM9" t="inlineStr">
         <is>
-          <t>21,53038;31,11519;41,8413;22,315;32,315;42,315</t>
+          <t>21,95876;31,0;41,11962;22,614;32,0;42,503</t>
         </is>
       </c>
       <c r="AN9" t="inlineStr">
         <is>
-          <t>21,26519;31,5759;41,4206;22,157;32,157;42,157</t>
+          <t>21,83567;31,0;41,0;22,612;32,0;42,0</t>
         </is>
       </c>
       <c r="AO9" t="inlineStr">
         <is>
-          <t>21,7353;31,1283;41,1144;22,280;32,280;42,280</t>
+          <t>21,9251;31,1081;41,1150;22,364;32,196;42,298</t>
         </is>
       </c>
       <c r="AP9" t="inlineStr">
         <is>
-          <t>21,7353;31,1283;41,1144;22,280;32,280;42,280</t>
+          <t>21,12682;31,0;41,1577;22,546;32,0;42,447</t>
         </is>
       </c>
       <c r="AQ9" t="inlineStr">
         <is>
-          <t>21,3676;31,641;41,572;22,140;32,140;42,140</t>
+          <t>21,11054;31,0;41,0;22,546;32,0;42,0</t>
         </is>
       </c>
     </row>
@@ -6251,141 +6251,141 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>60199</v>
+        <v>78676</v>
       </c>
       <c r="C10" t="n">
-        <v>13075</v>
+        <v>9200</v>
       </c>
       <c r="D10" t="n">
-        <v>9266</v>
+        <v>9816</v>
       </c>
       <c r="E10" t="n">
+        <v>435</v>
+      </c>
+      <c r="F10" t="n">
+        <v>234</v>
+      </c>
+      <c r="G10" t="n">
+        <v>357</v>
+      </c>
+      <c r="H10" t="n">
+        <v>107861</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>13457</v>
+      </c>
+      <c r="K10" t="n">
+        <v>653</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>535</v>
+      </c>
+      <c r="N10" t="n">
+        <v>94013</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>651</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0</v>
+      </c>
+      <c r="T10" t="n">
+        <v>10016</v>
+      </c>
+      <c r="U10" t="n">
+        <v>1171</v>
+      </c>
+      <c r="V10" t="n">
+        <v>1261</v>
+      </c>
+      <c r="W10" t="n">
+        <v>409</v>
+      </c>
+      <c r="X10" t="n">
+        <v>220</v>
+      </c>
+      <c r="Y10" t="n">
         <v>335</v>
       </c>
-      <c r="F10" t="n">
-        <v>335</v>
-      </c>
-      <c r="G10" t="n">
-        <v>335</v>
-      </c>
-      <c r="H10" t="n">
-        <v>60199</v>
-      </c>
-      <c r="I10" t="n">
-        <v>13075</v>
-      </c>
-      <c r="J10" t="n">
-        <v>9266</v>
-      </c>
-      <c r="K10" t="n">
-        <v>335</v>
-      </c>
-      <c r="L10" t="n">
-        <v>335</v>
-      </c>
-      <c r="M10" t="n">
-        <v>335</v>
-      </c>
-      <c r="N10" t="n">
-        <v>30099</v>
-      </c>
-      <c r="O10" t="n">
-        <v>6537</v>
-      </c>
-      <c r="P10" t="n">
-        <v>4633</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>167</v>
-      </c>
-      <c r="R10" t="n">
-        <v>167</v>
-      </c>
-      <c r="S10" t="n">
-        <v>167</v>
-      </c>
-      <c r="T10" t="n">
-        <v>7961</v>
-      </c>
-      <c r="U10" t="n">
-        <v>1389</v>
-      </c>
-      <c r="V10" t="n">
-        <v>1254</v>
-      </c>
-      <c r="W10" t="n">
-        <v>315</v>
-      </c>
-      <c r="X10" t="n">
-        <v>315</v>
-      </c>
-      <c r="Y10" t="n">
-        <v>315</v>
-      </c>
       <c r="Z10" t="n">
-        <v>7961</v>
+        <v>13732</v>
       </c>
       <c r="AA10" t="n">
-        <v>1389</v>
+        <v>0</v>
       </c>
       <c r="AB10" t="n">
-        <v>1254</v>
+        <v>1729</v>
       </c>
       <c r="AC10" t="n">
-        <v>315</v>
+        <v>614</v>
       </c>
       <c r="AD10" t="n">
-        <v>315</v>
+        <v>0</v>
       </c>
       <c r="AE10" t="n">
-        <v>315</v>
+        <v>503</v>
       </c>
       <c r="AF10" t="n">
-        <v>3980</v>
+        <v>11969</v>
       </c>
       <c r="AG10" t="n">
-        <v>694</v>
+        <v>0</v>
       </c>
       <c r="AH10" t="n">
-        <v>627</v>
+        <v>0</v>
       </c>
       <c r="AI10" t="n">
-        <v>157</v>
+        <v>612</v>
       </c>
       <c r="AJ10" t="n">
-        <v>157</v>
+        <v>0</v>
       </c>
       <c r="AK10" t="n">
-        <v>157</v>
+        <v>0</v>
       </c>
       <c r="AL10" t="inlineStr">
         <is>
-          <t>21,60199;31,13075;41,9266;22,335;32,335;42,335</t>
+          <t>21,78676;31,9200;41,9816;22,435;32,234;42,357</t>
         </is>
       </c>
       <c r="AM10" t="inlineStr">
         <is>
-          <t>21,60199;31,13075;41,9266;22,335;32,335;42,335</t>
+          <t>21,107861;31,0;41,13457;22,653;32,0;42,535</t>
         </is>
       </c>
       <c r="AN10" t="inlineStr">
         <is>
-          <t>21,30099;31,6537;41,4633;22,167;32,167;42,167</t>
+          <t>21,94013;31,0;41,0;22,651;32,0;42,0</t>
         </is>
       </c>
       <c r="AO10" t="inlineStr">
         <is>
-          <t>21,7961;31,1389;41,1254;22,315;32,315;42,315</t>
+          <t>21,10016;31,1171;41,1261;22,409;32,220;42,335</t>
         </is>
       </c>
       <c r="AP10" t="inlineStr">
         <is>
-          <t>21,7961;31,1389;41,1254;22,315;32,315;42,315</t>
+          <t>21,13732;31,0;41,1729;22,614;32,0;42,503</t>
         </is>
       </c>
       <c r="AQ10" t="inlineStr">
         <is>
-          <t>21,3980;31,694;41,627;22,157;32,157;42,157</t>
+          <t>21,11969;31,0;41,0;22,612;32,0;42,0</t>
         </is>
       </c>
     </row>
@@ -6394,141 +6394,141 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>67245</v>
+        <v>87418</v>
       </c>
       <c r="C11" t="n">
-        <v>14605</v>
+        <v>10223</v>
       </c>
       <c r="D11" t="n">
-        <v>10226</v>
+        <v>10907</v>
       </c>
       <c r="E11" t="n">
-        <v>350</v>
+        <v>455</v>
       </c>
       <c r="F11" t="n">
-        <v>350</v>
+        <v>244</v>
       </c>
       <c r="G11" t="n">
-        <v>350</v>
+        <v>373</v>
       </c>
       <c r="H11" t="n">
-        <v>67245</v>
+        <v>119846</v>
       </c>
       <c r="I11" t="n">
-        <v>14605</v>
+        <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>10226</v>
+        <v>14953</v>
       </c>
       <c r="K11" t="n">
-        <v>350</v>
+        <v>682</v>
       </c>
       <c r="L11" t="n">
-        <v>350</v>
+        <v>0</v>
       </c>
       <c r="M11" t="n">
-        <v>350</v>
+        <v>559</v>
       </c>
       <c r="N11" t="n">
-        <v>33622</v>
+        <v>104459</v>
       </c>
       <c r="O11" t="n">
-        <v>7302</v>
+        <v>0</v>
       </c>
       <c r="P11" t="n">
-        <v>5113</v>
+        <v>0</v>
       </c>
       <c r="Q11" t="n">
-        <v>175</v>
+        <v>682</v>
       </c>
       <c r="R11" t="n">
-        <v>175</v>
+        <v>0</v>
       </c>
       <c r="S11" t="n">
-        <v>175</v>
+        <v>0</v>
       </c>
       <c r="T11" t="n">
-        <v>8582</v>
+        <v>10799</v>
       </c>
       <c r="U11" t="n">
-        <v>1497</v>
+        <v>1262</v>
       </c>
       <c r="V11" t="n">
-        <v>1368</v>
+        <v>1375</v>
       </c>
       <c r="W11" t="n">
-        <v>350</v>
+        <v>455</v>
       </c>
       <c r="X11" t="n">
-        <v>350</v>
+        <v>244</v>
       </c>
       <c r="Y11" t="n">
-        <v>350</v>
+        <v>373</v>
       </c>
       <c r="Z11" t="n">
-        <v>8582</v>
+        <v>14805</v>
       </c>
       <c r="AA11" t="n">
-        <v>1497</v>
+        <v>0</v>
       </c>
       <c r="AB11" t="n">
-        <v>1368</v>
+        <v>1885</v>
       </c>
       <c r="AC11" t="n">
-        <v>350</v>
+        <v>682</v>
       </c>
       <c r="AD11" t="n">
-        <v>350</v>
+        <v>0</v>
       </c>
       <c r="AE11" t="n">
-        <v>350</v>
+        <v>559</v>
       </c>
       <c r="AF11" t="n">
-        <v>4291</v>
+        <v>12904</v>
       </c>
       <c r="AG11" t="n">
-        <v>748</v>
+        <v>0</v>
       </c>
       <c r="AH11" t="n">
-        <v>684</v>
+        <v>0</v>
       </c>
       <c r="AI11" t="n">
-        <v>175</v>
+        <v>682</v>
       </c>
       <c r="AJ11" t="n">
-        <v>175</v>
+        <v>0</v>
       </c>
       <c r="AK11" t="n">
-        <v>175</v>
+        <v>0</v>
       </c>
       <c r="AL11" t="inlineStr">
         <is>
-          <t>21,67245;31,14605;41,10226;22,350;32,350;42,350</t>
+          <t>21,87418;31,10223;41,10907;22,455;32,244;42,373</t>
         </is>
       </c>
       <c r="AM11" t="inlineStr">
         <is>
-          <t>21,67245;31,14605;41,10226;22,350;32,350;42,350</t>
+          <t>21,119846;31,0;41,14953;22,682;32,0;42,559</t>
         </is>
       </c>
       <c r="AN11" t="inlineStr">
         <is>
-          <t>21,33622;31,7302;41,5113;22,175;32,175;42,175</t>
+          <t>21,104459;31,0;41,0;22,682;32,0;42,0</t>
         </is>
       </c>
       <c r="AO11" t="inlineStr">
         <is>
-          <t>21,8582;31,1497;41,1368;22,350;32,350;42,350</t>
+          <t>21,10799;31,1262;41,1375;22,455;32,244;42,373</t>
         </is>
       </c>
       <c r="AP11" t="inlineStr">
         <is>
-          <t>21,8582;31,1497;41,1368;22,350;32,350;42,350</t>
+          <t>21,14805;31,0;41,1885;22,682;32,0;42,559</t>
         </is>
       </c>
       <c r="AQ11" t="inlineStr">
         <is>
-          <t>21,4291;31,748;41,684;22,175;32,175;42,175</t>
+          <t>21,12904;31,0;41,0;22,682;32,0;42,0</t>
         </is>
       </c>
     </row>
@@ -6839,13 +6839,13 @@
         </is>
       </c>
       <c r="T2" t="n">
-        <v>5619738.3248014</v>
+        <v>5863261.508827101</v>
       </c>
       <c r="U2" t="n">
-        <v>842234.0556</v>
+        <v>870639.49775664</v>
       </c>
       <c r="V2" t="n">
-        <v>856793.1760505</v>
+        <v>887162.35298315</v>
       </c>
       <c r="W2" t="n">
         <v>1940</v>
@@ -6886,8 +6886,16 @@
       <c r="AI2" t="n">
         <v>0</v>
       </c>
-      <c r="AJ2" t="inlineStr"/>
-      <c r="AK2" t="inlineStr"/>
+      <c r="AJ2" t="inlineStr">
+        <is>
+          <t>21,353832;31,0;41,44120</t>
+        </is>
+      </c>
+      <c r="AK2" t="inlineStr">
+        <is>
+          <t>21,338445;31,0;41,0</t>
+        </is>
+      </c>
       <c r="AL2" t="n">
         <v>11573665.886915</v>
       </c>
@@ -6907,10 +6915,10 @@
         <v>0</v>
       </c>
       <c r="AR2" t="n">
-        <v>0</v>
+        <v>614143.5022692536</v>
       </c>
       <c r="AS2" t="n">
-        <v>16373547.07073178</v>
+        <v>16987690.57300103</v>
       </c>
     </row>
     <row r="3">
@@ -6974,13 +6982,13 @@
         </is>
       </c>
       <c r="T3" t="n">
-        <v>719159.3037503</v>
+        <v>747538.31293795</v>
       </c>
       <c r="U3" t="n">
-        <v>112653.9772</v>
+        <v>115963.62464368</v>
       </c>
       <c r="V3" t="n">
-        <v>115512.1140265</v>
+        <v>119124.58871195</v>
       </c>
       <c r="W3" t="n">
         <v>1940</v>
@@ -7021,8 +7029,16 @@
       <c r="AI3" t="n">
         <v>0</v>
       </c>
-      <c r="AJ3" t="inlineStr"/>
-      <c r="AK3" t="inlineStr"/>
+      <c r="AJ3" t="inlineStr">
+        <is>
+          <t>21,41155;31,0;41,5238</t>
+        </is>
+      </c>
+      <c r="AK3" t="inlineStr">
+        <is>
+          <t>21,39254;31,0;41,0</t>
+        </is>
+      </c>
       <c r="AL3" t="n">
         <v>1311165.690855</v>
       </c>
@@ -7042,10 +7058,10 @@
         <v>0</v>
       </c>
       <c r="AR3" t="n">
-        <v>0</v>
+        <v>71987.30599037951</v>
       </c>
       <c r="AS3" t="n">
-        <v>2176499.402082675</v>
+        <v>2248486.708073054</v>
       </c>
     </row>
     <row r="4">
@@ -7514,13 +7530,13 @@
         </is>
       </c>
       <c r="T7" t="n">
-        <v>57380.7284</v>
+        <v>66313.88258768</v>
       </c>
       <c r="U7" t="n">
-        <v>10457.55</v>
+        <v>11503.23114</v>
       </c>
       <c r="V7" t="n">
-        <v>5751.74</v>
+        <v>6858.530508</v>
       </c>
       <c r="W7" t="n">
         <v>900</v>
@@ -7561,8 +7577,16 @@
       <c r="AI7" t="n">
         <v>0</v>
       </c>
-      <c r="AJ7" t="inlineStr"/>
-      <c r="AK7" t="inlineStr"/>
+      <c r="AJ7" t="inlineStr">
+        <is>
+          <t>21,12272;31,0;41,1520</t>
+        </is>
+      </c>
+      <c r="AK7" t="inlineStr">
+        <is>
+          <t>21,10733;31,0;41,0</t>
+        </is>
+      </c>
       <c r="AL7" t="n">
         <v>119121.8284</v>
       </c>
@@ -7582,10 +7606,10 @@
         <v>0</v>
       </c>
       <c r="AR7" t="n">
-        <v>0</v>
+        <v>22512.39947468</v>
       </c>
       <c r="AS7" t="n">
-        <v>167415.8284</v>
+        <v>189928.22787468</v>
       </c>
     </row>
     <row r="8">
@@ -7649,13 +7673,13 @@
         </is>
       </c>
       <c r="T8" t="n">
-        <v>57787.2084124</v>
+        <v>75654.51678776</v>
       </c>
       <c r="U8" t="n">
-        <v>10457.55</v>
+        <v>12548.91228</v>
       </c>
       <c r="V8" t="n">
-        <v>5795.715139999999</v>
+        <v>8010.69593</v>
       </c>
       <c r="W8" t="n">
         <v>900</v>
@@ -7696,8 +7720,16 @@
       <c r="AI8" t="n">
         <v>0</v>
       </c>
-      <c r="AJ8" t="inlineStr"/>
-      <c r="AK8" t="inlineStr"/>
+      <c r="AJ8" t="inlineStr">
+        <is>
+          <t>21,24545;31,0;41,3040</t>
+        </is>
+      </c>
+      <c r="AK8" t="inlineStr">
+        <is>
+          <t>21,21467;31,0;41,0</t>
+        </is>
+      </c>
       <c r="AL8" t="n">
         <v>119121.8284</v>
       </c>
@@ -7717,10 +7749,10 @@
         <v>0</v>
       </c>
       <c r="AR8" t="n">
-        <v>0</v>
+        <v>45033.84764986</v>
       </c>
       <c r="AS8" t="n">
-        <v>168075.1654674</v>
+        <v>213109.01311726</v>
       </c>
     </row>
     <row r="9">
@@ -7919,13 +7951,13 @@
         </is>
       </c>
       <c r="T10" t="n">
-        <v>241001.1975318</v>
+        <v>250610.31565956</v>
       </c>
       <c r="U10" t="n">
-        <v>42998</v>
+        <v>44120.8756</v>
       </c>
       <c r="V10" t="n">
-        <v>27852.9347573</v>
+        <v>29031.75347736</v>
       </c>
       <c r="W10" t="n">
         <v>1940</v>
@@ -7966,8 +7998,16 @@
       <c r="AI10" t="n">
         <v>0</v>
       </c>
-      <c r="AJ10" t="inlineStr"/>
-      <c r="AK10" t="inlineStr"/>
+      <c r="AJ10" t="inlineStr">
+        <is>
+          <t>21,13286;31,0;41,1628</t>
+        </is>
+      </c>
+      <c r="AK10" t="inlineStr">
+        <is>
+          <t>21,11747;31,0;41,0</t>
+        </is>
+      </c>
       <c r="AL10" t="n">
         <v>537954.151025</v>
       </c>
@@ -7987,10 +8027,10 @@
         <v>0</v>
       </c>
       <c r="AR10" t="n">
-        <v>0</v>
+        <v>24135.167408105</v>
       </c>
       <c r="AS10" t="n">
-        <v>709154.772386275</v>
+        <v>733289.93979438</v>
       </c>
     </row>
     <row r="11">
@@ -8054,13 +8094,13 @@
         </is>
       </c>
       <c r="T11" t="n">
-        <v>259365.2348498</v>
+        <v>307414.8254886</v>
       </c>
       <c r="U11" t="n">
-        <v>42998</v>
+        <v>48613.378</v>
       </c>
       <c r="V11" t="n">
-        <v>30179.1393303</v>
+        <v>36082.57712489</v>
       </c>
       <c r="W11" t="n">
         <v>1940</v>
@@ -8101,8 +8141,16 @@
       <c r="AI11" t="n">
         <v>0</v>
       </c>
-      <c r="AJ11" t="inlineStr"/>
-      <c r="AK11" t="inlineStr"/>
+      <c r="AJ11" t="inlineStr">
+        <is>
+          <t>21,66433;31,0;41,8150</t>
+        </is>
+      </c>
+      <c r="AK11" t="inlineStr">
+        <is>
+          <t>21,58739;31,0;41,0</t>
+        </is>
+      </c>
       <c r="AL11" t="n">
         <v>537954.151025</v>
       </c>
@@ -8122,10 +8170,10 @@
         <v>0</v>
       </c>
       <c r="AR11" t="n">
-        <v>0</v>
+        <v>120740.4661576925</v>
       </c>
       <c r="AS11" t="n">
-        <v>741290.4859990251</v>
+        <v>862030.9521567175</v>
       </c>
     </row>
     <row r="12">
@@ -8189,13 +8237,13 @@
         </is>
       </c>
       <c r="T12" t="n">
-        <v>277729.2721678</v>
+        <v>325778.8628066</v>
       </c>
       <c r="U12" t="n">
-        <v>42998</v>
+        <v>48613.378</v>
       </c>
       <c r="V12" t="n">
-        <v>32505.3439033</v>
+        <v>38408.78169788999</v>
       </c>
       <c r="W12" t="n">
         <v>1940</v>
@@ -8236,8 +8284,16 @@
       <c r="AI12" t="n">
         <v>0</v>
       </c>
-      <c r="AJ12" t="inlineStr"/>
-      <c r="AK12" t="inlineStr"/>
+      <c r="AJ12" t="inlineStr">
+        <is>
+          <t>21,66433;31,0;41,8150</t>
+        </is>
+      </c>
+      <c r="AK12" t="inlineStr">
+        <is>
+          <t>21,58739;31,0;41,0</t>
+        </is>
+      </c>
       <c r="AL12" t="n">
         <v>537954.151025</v>
       </c>
@@ -8257,10 +8313,10 @@
         <v>0</v>
       </c>
       <c r="AR12" t="n">
-        <v>0</v>
+        <v>120740.4661576925</v>
       </c>
       <c r="AS12" t="n">
-        <v>773426.1996117749</v>
+        <v>894166.6657694674</v>
       </c>
     </row>
     <row r="13">
@@ -8324,13 +8380,13 @@
         </is>
       </c>
       <c r="T13" t="n">
-        <v>296093.3094858</v>
+        <v>391107.3431037</v>
       </c>
       <c r="U13" t="n">
-        <v>42998</v>
+        <v>54100.0588</v>
       </c>
       <c r="V13" t="n">
-        <v>34831.5484763</v>
+        <v>46527.34329969</v>
       </c>
       <c r="W13" t="n">
         <v>1940</v>
@@ -8371,8 +8427,16 @@
       <c r="AI13" t="n">
         <v>0</v>
       </c>
-      <c r="AJ13" t="inlineStr"/>
-      <c r="AK13" t="inlineStr"/>
+      <c r="AJ13" t="inlineStr">
+        <is>
+          <t>21,131231;31,0;41,16135</t>
+        </is>
+      </c>
+      <c r="AK13" t="inlineStr">
+        <is>
+          <t>21,115844;31,0;41,0</t>
+        </is>
+      </c>
       <c r="AL13" t="n">
         <v>537954.151025</v>
       </c>
@@ -8392,10 +8456,10 @@
         <v>0</v>
       </c>
       <c r="AR13" t="n">
-        <v>0</v>
+        <v>238869.0595723925</v>
       </c>
       <c r="AS13" t="n">
-        <v>805561.9132245251</v>
+        <v>1044430.972796917</v>
       </c>
     </row>
     <row r="14">
@@ -8459,13 +8523,13 @@
         </is>
       </c>
       <c r="T14" t="n">
-        <v>296093.3094858</v>
+        <v>344142.9001246</v>
       </c>
       <c r="U14" t="n">
-        <v>42998</v>
+        <v>48613.378</v>
       </c>
       <c r="V14" t="n">
-        <v>34831.5484763</v>
+        <v>40734.98627089</v>
       </c>
       <c r="W14" t="n">
         <v>1940</v>
@@ -8506,8 +8570,16 @@
       <c r="AI14" t="n">
         <v>0</v>
       </c>
-      <c r="AJ14" t="inlineStr"/>
-      <c r="AK14" t="inlineStr"/>
+      <c r="AJ14" t="inlineStr">
+        <is>
+          <t>21,66433;31,0;41,8150</t>
+        </is>
+      </c>
+      <c r="AK14" t="inlineStr">
+        <is>
+          <t>21,58739;31,0;41,0</t>
+        </is>
+      </c>
       <c r="AL14" t="n">
         <v>537954.151025</v>
       </c>
@@ -8527,10 +8599,10 @@
         <v>0</v>
       </c>
       <c r="AR14" t="n">
-        <v>0</v>
+        <v>120740.4661576925</v>
       </c>
       <c r="AS14" t="n">
-        <v>805323.9132245251</v>
+        <v>926064.3793822175</v>
       </c>
     </row>
     <row r="15">
@@ -8594,13 +8666,13 @@
         </is>
       </c>
       <c r="T15" t="n">
-        <v>442561.49225</v>
+        <v>502810.78245</v>
       </c>
       <c r="U15" t="n">
-        <v>64410.5918</v>
+        <v>71452.11214224</v>
       </c>
       <c r="V15" t="n">
-        <v>59695.1493648</v>
+        <v>67144.50679120001</v>
       </c>
       <c r="W15" t="n">
         <v>1940</v>
@@ -8641,8 +8713,16 @@
       <c r="AI15" t="n">
         <v>0</v>
       </c>
-      <c r="AJ15" t="inlineStr"/>
-      <c r="AK15" t="inlineStr"/>
+      <c r="AJ15" t="inlineStr">
+        <is>
+          <t>21,83605;31,0;41,10330</t>
+        </is>
+      </c>
+      <c r="AK15" t="inlineStr">
+        <is>
+          <t>21,74373;31,0;41,0</t>
+        </is>
+      </c>
       <c r="AL15" t="n">
         <v>828093.75702</v>
       </c>
@@ -8662,10 +8742,10 @@
         <v>0</v>
       </c>
       <c r="AR15" t="n">
-        <v>0</v>
+        <v>151669.585763256</v>
       </c>
       <c r="AS15" t="n">
-        <v>1242980.6845176</v>
+        <v>1394650.270280856</v>
       </c>
     </row>
     <row r="16">
@@ -8729,13 +8809,13 @@
         </is>
       </c>
       <c r="T16" t="n">
-        <v>442561.49225</v>
+        <v>512852.66415</v>
       </c>
       <c r="U16" t="n">
-        <v>64410.5918</v>
+        <v>72626.53219928</v>
       </c>
       <c r="V16" t="n">
-        <v>59695.1493648</v>
+        <v>68387.17490624</v>
       </c>
       <c r="W16" t="n">
         <v>1940</v>
@@ -8776,8 +8856,16 @@
       <c r="AI16" t="n">
         <v>0</v>
       </c>
-      <c r="AJ16" t="inlineStr"/>
-      <c r="AK16" t="inlineStr"/>
+      <c r="AJ16" t="inlineStr">
+        <is>
+          <t>21,97540;31,0;41,12054</t>
+        </is>
+      </c>
+      <c r="AK16" t="inlineStr">
+        <is>
+          <t>21,86769;31,0;41,0</t>
+        </is>
+      </c>
       <c r="AL16" t="n">
         <v>828093.75702</v>
       </c>
@@ -8797,10 +8885,10 @@
         <v>0</v>
       </c>
       <c r="AR16" t="n">
-        <v>0</v>
+        <v>176960.307518312</v>
       </c>
       <c r="AS16" t="n">
-        <v>1243218.6845176</v>
+        <v>1420178.992035912</v>
       </c>
     </row>
     <row r="17">
@@ -8864,13 +8952,13 @@
         </is>
       </c>
       <c r="T17" t="n">
-        <v>1118406.0036521</v>
+        <v>1210982.98795439</v>
       </c>
       <c r="U17" t="n">
-        <v>155629.9848</v>
+        <v>166449.7664656</v>
       </c>
       <c r="V17" t="n">
-        <v>176291.2656</v>
+        <v>188008.5392</v>
       </c>
       <c r="W17" t="n">
         <v>1940</v>
@@ -8911,8 +8999,16 @@
       <c r="AI17" t="n">
         <v>0</v>
       </c>
-      <c r="AJ17" t="inlineStr"/>
-      <c r="AK17" t="inlineStr"/>
+      <c r="AJ17" t="inlineStr">
+        <is>
+          <t>21,129868;31,0;41,16454</t>
+        </is>
+      </c>
+      <c r="AK17" t="inlineStr">
+        <is>
+          <t>21,117448;31,0;41,0</t>
+        </is>
+      </c>
       <c r="AL17" t="n">
         <v>1896601.19322</v>
       </c>
@@ -8932,10 +9028,10 @@
         <v>0</v>
       </c>
       <c r="AR17" t="n">
-        <v>0</v>
+        <v>234607.80099493</v>
       </c>
       <c r="AS17" t="n">
-        <v>3219856.6759721</v>
+        <v>3454464.47696703</v>
       </c>
     </row>
     <row r="18">
@@ -8999,13 +9095,13 @@
         </is>
       </c>
       <c r="T18" t="n">
-        <v>5619738.3248014</v>
+        <v>5863261.508827101</v>
       </c>
       <c r="U18" t="n">
-        <v>842234.0556</v>
+        <v>870639.49775664</v>
       </c>
       <c r="V18" t="n">
-        <v>856793.1760505</v>
+        <v>887162.35298315</v>
       </c>
       <c r="W18" t="n">
         <v>1940</v>
@@ -9046,8 +9142,16 @@
       <c r="AI18" t="n">
         <v>0</v>
       </c>
-      <c r="AJ18" t="inlineStr"/>
-      <c r="AK18" t="inlineStr"/>
+      <c r="AJ18" t="inlineStr">
+        <is>
+          <t>21,353832;31,0;41,44120</t>
+        </is>
+      </c>
+      <c r="AK18" t="inlineStr">
+        <is>
+          <t>21,338445;31,0;41,0</t>
+        </is>
+      </c>
       <c r="AL18" t="n">
         <v>11573665.886915</v>
       </c>
@@ -9067,10 +9171,10 @@
         <v>0</v>
       </c>
       <c r="AR18" t="n">
-        <v>0</v>
+        <v>614143.5022692536</v>
       </c>
       <c r="AS18" t="n">
-        <v>16373547.07073178</v>
+        <v>16987690.57300103</v>
       </c>
     </row>
     <row r="19">
@@ -9134,13 +9238,13 @@
         </is>
       </c>
       <c r="T19" t="n">
-        <v>9286610.202018701</v>
+        <v>9530133.3860444</v>
       </c>
       <c r="U19" t="n">
-        <v>1388751.1924</v>
+        <v>1417156.63455664</v>
       </c>
       <c r="V19" t="n">
-        <v>1408525.555766</v>
+        <v>1438894.73269865</v>
       </c>
       <c r="W19" t="n">
         <v>1940</v>
@@ -9181,8 +9285,16 @@
       <c r="AI19" t="n">
         <v>0</v>
       </c>
-      <c r="AJ19" t="inlineStr"/>
-      <c r="AK19" t="inlineStr"/>
+      <c r="AJ19" t="inlineStr">
+        <is>
+          <t>21,353832;31,0;41,44120</t>
+        </is>
+      </c>
+      <c r="AK19" t="inlineStr">
+        <is>
+          <t>21,338445;31,0;41,0</t>
+        </is>
+      </c>
       <c r="AL19" t="n">
         <v>18781732.93276</v>
       </c>
@@ -9202,10 +9314,10 @@
         <v>0</v>
       </c>
       <c r="AR19" t="n">
-        <v>0</v>
+        <v>614143.5022692536</v>
       </c>
       <c r="AS19" t="n">
-        <v>26986942.3752332</v>
+        <v>27601085.87750245</v>
       </c>
     </row>
     <row r="20">
@@ -9269,13 +9381,13 @@
         </is>
       </c>
       <c r="T20" t="n">
-        <v>209768.4766811</v>
+        <v>215093.21619155</v>
       </c>
       <c r="U20" t="n">
-        <v>43250.7886</v>
+        <v>43903.34169264</v>
       </c>
       <c r="V20" t="n">
-        <v>24003.495004</v>
+        <v>24517.5572508</v>
       </c>
       <c r="W20" t="n">
         <v>900</v>
@@ -9316,8 +9428,16 @@
       <c r="AI20" t="n">
         <v>0</v>
       </c>
-      <c r="AJ20" t="inlineStr"/>
-      <c r="AK20" t="inlineStr"/>
+      <c r="AJ20" t="inlineStr">
+        <is>
+          <t>21,7410;31,0;41,714</t>
+        </is>
+      </c>
+      <c r="AK20" t="inlineStr">
+        <is>
+          <t>21,6576;31,0;41,0</t>
+        </is>
+      </c>
       <c r="AL20" t="n">
         <v>568353.7644400001</v>
       </c>
@@ -9337,10 +9457,10 @@
         <v>0</v>
       </c>
       <c r="AR20" t="n">
-        <v>0</v>
+        <v>12783.213768766</v>
       </c>
       <c r="AS20" t="n">
-        <v>651024.5142941</v>
+        <v>663807.728062866</v>
       </c>
     </row>
     <row r="21">
@@ -9404,13 +9524,13 @@
         </is>
       </c>
       <c r="T21" t="n">
-        <v>286647.4124342</v>
+        <v>293728.10962702</v>
       </c>
       <c r="U21" t="n">
-        <v>51120.9912</v>
+        <v>51965.43115688</v>
       </c>
       <c r="V21" t="n">
-        <v>35119.452009</v>
+        <v>35857.6605236</v>
       </c>
       <c r="W21" t="n">
         <v>1100</v>
@@ -9451,8 +9571,16 @@
       <c r="AI21" t="n">
         <v>0</v>
       </c>
-      <c r="AJ21" t="inlineStr"/>
-      <c r="AK21" t="inlineStr"/>
+      <c r="AJ21" t="inlineStr">
+        <is>
+          <t>21,9939;31,0;41,1037</t>
+        </is>
+      </c>
+      <c r="AK21" t="inlineStr">
+        <is>
+          <t>21,9022;31,0;41,0</t>
+        </is>
+      </c>
       <c r="AL21" t="n">
         <v>672828.2412299999</v>
       </c>
@@ -9472,10 +9600,10 @@
         <v>0</v>
       </c>
       <c r="AR21" t="n">
-        <v>0</v>
+        <v>17152.031854242</v>
       </c>
       <c r="AS21" t="n">
-        <v>848629.85076595</v>
+        <v>865781.882620192</v>
       </c>
     </row>
     <row r="22">
@@ -9539,13 +9667,13 @@
         </is>
       </c>
       <c r="T22" t="n">
-        <v>414328.5086642</v>
+        <v>427443.68351934</v>
       </c>
       <c r="U22" t="n">
-        <v>65190.35</v>
+        <v>66714.39327</v>
       </c>
       <c r="V22" t="n">
-        <v>54470.6528851</v>
+        <v>56011.50710416</v>
       </c>
       <c r="W22" t="n">
         <v>1940</v>
@@ -9586,8 +9714,16 @@
       <c r="AI22" t="n">
         <v>0</v>
       </c>
-      <c r="AJ22" t="inlineStr"/>
-      <c r="AK22" t="inlineStr"/>
+      <c r="AJ22" t="inlineStr">
+        <is>
+          <t>21,18747;31,0;41,2199</t>
+        </is>
+      </c>
+      <c r="AK22" t="inlineStr">
+        <is>
+          <t>21,17416;31,0;41,0</t>
+        </is>
+      </c>
       <c r="AL22" t="n">
         <v>851233.3802750001</v>
       </c>
@@ -9607,10 +9743,10 @@
         <v>0</v>
       </c>
       <c r="AR22" t="n">
-        <v>0</v>
+        <v>32490.985177735</v>
       </c>
       <c r="AS22" t="n">
-        <v>1189453.177753525</v>
+        <v>1221944.16293126</v>
       </c>
     </row>
     <row r="23">
@@ -9674,13 +9810,13 @@
         </is>
       </c>
       <c r="T23" t="n">
-        <v>489410.762125</v>
+        <v>506620.1972</v>
       </c>
       <c r="U23" t="n">
-        <v>72804.31140000001</v>
+        <v>74809.96862494001</v>
       </c>
       <c r="V23" t="n">
-        <v>67562.0304536</v>
+        <v>69636.38742216</v>
       </c>
       <c r="W23" t="n">
         <v>1940</v>
@@ -9721,8 +9857,16 @@
       <c r="AI23" t="n">
         <v>0</v>
       </c>
-      <c r="AJ23" t="inlineStr"/>
-      <c r="AK23" t="inlineStr"/>
+      <c r="AJ23" t="inlineStr">
+        <is>
+          <t>21,24739;31,0;41,2979</t>
+        </is>
+      </c>
+      <c r="AK23" t="inlineStr">
+        <is>
+          <t>21,23216;31,0;41,0</t>
+        </is>
+      </c>
       <c r="AL23" t="n">
         <v>930059.11386</v>
       </c>
@@ -9742,10 +9886,10 @@
         <v>0</v>
       </c>
       <c r="AR23" t="n">
-        <v>0</v>
+        <v>42976.022496306</v>
       </c>
       <c r="AS23" t="n">
-        <v>1393219.1858932</v>
+        <v>1436195.208389506</v>
       </c>
     </row>
     <row r="24">
@@ -9809,13 +9953,13 @@
         </is>
       </c>
       <c r="T24" t="n">
-        <v>564520.25399</v>
+        <v>585193.260586</v>
       </c>
       <c r="U24" t="n">
-        <v>85924.1676</v>
+        <v>88339.32328496</v>
       </c>
       <c r="V24" t="n">
-        <v>83385.11634179999</v>
+        <v>85933.78559383999</v>
       </c>
       <c r="W24" t="n">
         <v>1940</v>
@@ -9856,8 +10000,16 @@
       <c r="AI24" t="n">
         <v>0</v>
       </c>
-      <c r="AJ24" t="inlineStr"/>
-      <c r="AK24" t="inlineStr"/>
+      <c r="AJ24" t="inlineStr">
+        <is>
+          <t>21,29815;31,0;41,3675</t>
+        </is>
+      </c>
+      <c r="AK24" t="inlineStr">
+        <is>
+          <t>21,28187;31,0;41,0</t>
+        </is>
+      </c>
       <c r="AL24" t="n">
         <v>1054171.10279</v>
       </c>
@@ -9877,10 +10029,10 @@
         <v>0</v>
       </c>
       <c r="AR24" t="n">
-        <v>0</v>
+        <v>51992.429021454</v>
       </c>
       <c r="AS24" t="n">
-        <v>1650790.42939535</v>
+        <v>1702782.858416804</v>
       </c>
     </row>
     <row r="25">
@@ -9944,13 +10096,13 @@
         </is>
       </c>
       <c r="T25" t="n">
-        <v>719159.3037503</v>
+        <v>747538.31293795</v>
       </c>
       <c r="U25" t="n">
-        <v>112653.9772</v>
+        <v>115963.62464368</v>
       </c>
       <c r="V25" t="n">
-        <v>115512.1140265</v>
+        <v>119124.58871195</v>
       </c>
       <c r="W25" t="n">
         <v>1940</v>
@@ -9991,8 +10143,16 @@
       <c r="AI25" t="n">
         <v>0</v>
       </c>
-      <c r="AJ25" t="inlineStr"/>
-      <c r="AK25" t="inlineStr"/>
+      <c r="AJ25" t="inlineStr">
+        <is>
+          <t>21,41155;31,0;41,5238</t>
+        </is>
+      </c>
+      <c r="AK25" t="inlineStr">
+        <is>
+          <t>21,39254;31,0;41,0</t>
+        </is>
+      </c>
       <c r="AL25" t="n">
         <v>1311165.690855</v>
       </c>
@@ -10012,10 +10172,10 @@
         <v>0</v>
       </c>
       <c r="AR25" t="n">
-        <v>0</v>
+        <v>71987.30599037951</v>
       </c>
       <c r="AS25" t="n">
-        <v>2176499.402082675</v>
+        <v>2248486.708073054</v>
       </c>
     </row>
   </sheetData>

</xml_diff>